<commit_message>
updated excel file - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/Java/Final Pro/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3664A1D-FE30-4645-B812-4BA6F309F348}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,8 +22,14 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="253">
   <si>
     <t>Initials</t>
   </si>
@@ -753,18 +758,60 @@
   </si>
   <si>
     <t>232-273</t>
+  </si>
+  <si>
+    <t>US21_check_Gender_Role</t>
+  </si>
+  <si>
+    <t>183-224</t>
+  </si>
+  <si>
+    <t>TestUS21CheckGenderRole.java</t>
+  </si>
+  <si>
+    <t>testGenderRoleHusband, testGenderRoleWife()</t>
+  </si>
+  <si>
+    <t>US22_check_Unique_FamilyId, foundADuplicateId</t>
+  </si>
+  <si>
+    <t>MultiIndividualFamilyData.java, FamilyTreeParser.java</t>
+  </si>
+  <si>
+    <t>231-252, 50-58</t>
+  </si>
+  <si>
+    <t>checkFamilyUniqueId, checkFamilyUniqueId2</t>
+  </si>
+  <si>
+    <t>TestUS22UniqueIds.java</t>
+  </si>
+  <si>
+    <t>Complete user stories earlier and on time</t>
+  </si>
+  <si>
+    <t>Reply to messaes on slack</t>
+  </si>
+  <si>
+    <t>Avoid inegration at the end</t>
+  </si>
+  <si>
+    <t>Avoid refactoring at the end</t>
+  </si>
+  <si>
+    <t>Late start of new things to be implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
     <numFmt numFmtId="166" formatCode="m&quot;-&quot;yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -967,7 +1014,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1048,7 +1095,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1061,10 +1108,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5185000000000006E-2"/>
-          <c:y val="5.4688500000000001E-2"/>
-          <c:w val="0.89981500000000003"/>
-          <c:h val="0.84428700000000001"/>
+          <c:x val="0.095185"/>
+          <c:y val="0.0546885"/>
+          <c:w val="0.899815"/>
+          <c:h val="0.844287"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1107,16 +1154,16 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42060</c:v>
+                  <c:v>42060.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42087</c:v>
+                  <c:v>42087.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,25 +1175,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4D8D-48F0-9F2D-0F8AAA21AC8A}"/>
             </c:ext>
@@ -1162,11 +1209,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:axId val="1041759056"/>
+        <c:axId val="1041746144"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="1041759056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,14 +1247,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="1041746144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="1041746144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1299,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="1041759056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1295,7 +1342,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1308,10 +1355,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.3853299999999997E-2"/>
-          <c:y val="5.4688500000000001E-2"/>
-          <c:w val="0.92114700000000005"/>
-          <c:h val="0.84428700000000001"/>
+          <c:x val="0.0738533"/>
+          <c:y val="0.0546885"/>
+          <c:w val="0.921147"/>
+          <c:h val="0.844287"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1357,13 +1404,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42059</c:v>
+                  <c:v>42059.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="m/d/yyyy">
-                  <c:v>42087</c:v>
+                <c:pt idx="2" formatCode="m/d/yy">
+                  <c:v>42087.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,19 +1422,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2690-4E11-B0A0-7E616747BB0B}"/>
             </c:ext>
@@ -1403,11 +1450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:axId val="1013530416"/>
+        <c:axId val="1013895728"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="1013530416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,14 +1488,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="1013895728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="1013895728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,11 +1540,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="1013530416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="8"/>
-        <c:minorUnit val="4"/>
+        <c:majorUnit val="8.0"/>
+        <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1555,7 +1602,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,7 +1638,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1599,8 +1646,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1336924" y="1432570"/>
-          <a:ext cx="1438826" cy="970570"/>
+          <a:off x="1275238" y="1447084"/>
+          <a:ext cx="1389841" cy="981456"/>
           <a:chOff x="-19049" y="-64007"/>
           <a:chExt cx="1389841" cy="981455"/>
         </a:xfrm>
@@ -1610,7 +1657,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1713,7 +1760,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1735,7 +1782,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -1861,7 +1908,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1869,8 +1916,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5635229" y="1427151"/>
-          <a:ext cx="1311367" cy="661502"/>
+          <a:off x="5263300" y="1441665"/>
+          <a:ext cx="1249682" cy="668759"/>
           <a:chOff x="-19050" y="-41148"/>
           <a:chExt cx="1249682" cy="668759"/>
         </a:xfrm>
@@ -1880,7 +1927,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1983,7 +2030,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2005,7 +2052,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2084,7 +2131,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2092,8 +2139,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2969441" y="1247346"/>
-          <a:ext cx="1130542" cy="909302"/>
+          <a:off x="2769870" y="1260046"/>
+          <a:ext cx="1063413" cy="920188"/>
           <a:chOff x="-19050" y="-52577"/>
           <a:chExt cx="1063412" cy="920188"/>
         </a:xfrm>
@@ -2103,7 +2150,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2206,7 +2253,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2228,7 +2275,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2307,7 +2354,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2315,8 +2362,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4097019" y="1580822"/>
-          <a:ext cx="431074" cy="623679"/>
+          <a:off x="3830319" y="1597151"/>
+          <a:ext cx="391160" cy="630936"/>
           <a:chOff x="-17779" y="-41148"/>
           <a:chExt cx="391159" cy="630936"/>
         </a:xfrm>
@@ -2326,7 +2373,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2429,7 +2476,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2451,7 +2498,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2577,7 +2624,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2585,8 +2632,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4524284" y="1268511"/>
-          <a:ext cx="1183761" cy="964844"/>
+          <a:off x="4217670" y="1281211"/>
+          <a:ext cx="1118446" cy="975730"/>
           <a:chOff x="-19050" y="-52577"/>
           <a:chExt cx="1118445" cy="975730"/>
         </a:xfrm>
@@ -2596,7 +2643,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2699,7 +2746,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2721,7 +2768,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2800,7 +2847,7 @@
         <xdr:cNvPr id="20" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2808,8 +2855,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5786293" y="5027903"/>
-          <a:ext cx="1287601" cy="861592"/>
+          <a:off x="5414364" y="5082332"/>
+          <a:ext cx="1225916" cy="872477"/>
           <a:chOff x="0" y="-41147"/>
           <a:chExt cx="1225916" cy="872477"/>
         </a:xfrm>
@@ -2819,7 +2866,7 @@
           <xdr:cNvPr id="18" name="Shape 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2922,7 +2969,7 @@
           <xdr:cNvPr id="19" name="Shape 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2944,7 +2991,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3028,7 +3075,7 @@
         <xdr:cNvPr id="22" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4153,21 +4200,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.86328125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" customWidth="1"/>
-    <col min="4" max="5" width="20.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4184,14 +4231,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -4208,7 +4255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -4225,7 +4272,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -4242,7 +4289,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4259,21 +4306,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4284,7 +4331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4301,16 +4348,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.19921875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
@@ -4318,7 +4365,7 @@
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -4335,7 +4382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4352,7 +4399,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4369,7 +4416,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4386,7 +4433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4403,7 +4450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4420,7 +4467,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -4437,7 +4484,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -4454,7 +4501,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4471,7 +4518,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -4488,7 +4535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -4505,7 +4552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -4522,7 +4569,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -4539,7 +4586,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -4552,7 +4599,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -4569,7 +4616,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -4586,7 +4633,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -4599,7 +4646,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -4616,7 +4663,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -4633,7 +4680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -4646,7 +4693,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -4659,7 +4706,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -4676,7 +4723,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -4693,7 +4740,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -4706,7 +4753,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -4723,7 +4770,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -4736,7 +4783,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>4</v>
       </c>
@@ -4749,7 +4796,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>4</v>
       </c>
@@ -4762,7 +4809,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -4775,7 +4822,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -4792,7 +4839,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>4</v>
       </c>
@@ -4805,7 +4852,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -4822,7 +4869,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>4</v>
       </c>
@@ -4835,7 +4882,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="14.15" customHeight="1">
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="28">
         <v>3</v>
       </c>
@@ -4862,23 +4909,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="9.46484375" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" customWidth="1"/>
-    <col min="7" max="256" width="10.86328125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" customHeight="1">
+    <row r="1" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4890,7 +4939,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="13" customHeight="1">
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -4902,7 +4951,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="13" customHeight="1">
+    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -4914,7 +4963,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="13" customHeight="1">
+    <row r="4" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4924,7 +4973,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="13" customHeight="1">
+    <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
@@ -4936,7 +4985,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="13" customHeight="1">
+    <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -4948,7 +4997,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="13" customHeight="1">
+    <row r="7" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4958,7 +5007,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="13" customHeight="1">
+    <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -4970,7 +5019,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="13" customHeight="1">
+    <row r="9" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4980,7 +5029,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="13" customHeight="1">
+    <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4990,7 +5039,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="13" customHeight="1">
+    <row r="11" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5000,7 +5049,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="13" customHeight="1">
+    <row r="12" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5010,7 +5059,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="13" customHeight="1">
+    <row r="13" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5020,7 +5069,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="13" customHeight="1">
+    <row r="14" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -5044,7 +5093,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1">
+    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -5062,7 +5111,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="13" customHeight="1">
+    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>113</v>
       </c>
@@ -5088,7 +5137,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="13" customHeight="1">
+    <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
@@ -5114,7 +5163,7 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="13" customHeight="1">
+    <row r="18" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -5138,7 +5187,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="13" customHeight="1">
+    <row r="19" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
@@ -5162,7 +5211,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="13" customHeight="1">
+    <row r="20" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="13"/>
@@ -5172,7 +5221,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13" customHeight="1">
+    <row r="21" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5182,7 +5231,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13" customHeight="1">
+    <row r="22" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5192,7 +5241,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="13" customHeight="1">
+    <row r="23" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5202,7 +5251,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="13" customHeight="1">
+    <row r="24" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5212,7 +5261,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="13" customHeight="1">
+    <row r="25" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5222,7 +5271,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="13" customHeight="1">
+    <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5232,7 +5281,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="13" customHeight="1">
+    <row r="27" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -5242,7 +5291,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="13" customHeight="1">
+    <row r="28" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -5252,7 +5301,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="13" customHeight="1">
+    <row r="29" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -5262,7 +5311,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="13" customHeight="1">
+    <row r="30" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5272,7 +5321,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="13" customHeight="1">
+    <row r="31" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -5282,7 +5331,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1">
+    <row r="32" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -5292,7 +5341,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="13" customHeight="1">
+    <row r="33" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -5302,7 +5351,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="13" customHeight="1">
+    <row r="34" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -5312,7 +5361,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="13" customHeight="1">
+    <row r="35" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -5322,7 +5371,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="13" customHeight="1">
+    <row r="36" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -5332,7 +5381,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="13" customHeight="1">
+    <row r="37" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -5342,7 +5391,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="13" customHeight="1">
+    <row r="38" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -5352,7 +5401,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="13" customHeight="1">
+    <row r="39" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -5373,23 +5422,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="4" width="7.19921875" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" customWidth="1"/>
-    <col min="7" max="256" width="10.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1">
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -5410,7 +5461,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1">
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15">
         <v>42046</v>
       </c>
@@ -5425,7 +5476,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="13" customHeight="1">
+    <row r="3" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15">
         <v>42059</v>
       </c>
@@ -5448,7 +5499,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="13" customHeight="1">
+    <row r="4" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>42087</v>
       </c>
@@ -5458,12 +5509,16 @@
       <c r="C4" s="4">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="4">
+        <v>256</v>
+      </c>
+      <c r="E4" s="4">
+        <v>305</v>
+      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="13" customHeight="1">
+    <row r="5" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5472,7 +5527,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="13" customHeight="1">
+    <row r="6" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5481,7 +5536,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="13" customHeight="1">
+    <row r="7" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5490,7 +5545,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="13" customHeight="1">
+    <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5499,7 +5554,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="13" customHeight="1">
+    <row r="9" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5508,7 +5563,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="13" customHeight="1">
+    <row r="10" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5517,7 +5572,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="13" customHeight="1">
+    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5526,7 +5581,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="13" customHeight="1">
+    <row r="12" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5535,7 +5590,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="13" customHeight="1">
+    <row r="13" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5544,7 +5599,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="13" customHeight="1">
+    <row r="14" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5553,7 +5608,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="13" customHeight="1">
+    <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5562,7 +5617,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="13" customHeight="1">
+    <row r="16" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5571,7 +5626,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="13" customHeight="1">
+    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -5580,7 +5635,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="13" customHeight="1">
+    <row r="18" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5589,7 +5644,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="13" customHeight="1">
+    <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -5598,7 +5653,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="13" customHeight="1">
+    <row r="20" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5607,7 +5662,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="13" customHeight="1">
+    <row r="21" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5616,7 +5671,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="13" customHeight="1">
+    <row r="22" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5625,7 +5680,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="13" customHeight="1">
+    <row r="23" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5634,7 +5689,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="13" customHeight="1">
+    <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5643,7 +5698,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="13" customHeight="1">
+    <row r="25" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5652,7 +5707,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="13" customHeight="1">
+    <row r="26" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5672,35 +5727,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q9"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="8.46484375" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.46484375" customWidth="1"/>
-    <col min="12" max="12" width="19.19921875" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.86328125" customWidth="1"/>
-    <col min="15" max="15" width="10.19921875" customWidth="1"/>
-    <col min="16" max="16" width="16.46484375" customWidth="1"/>
-    <col min="17" max="17" width="10.19921875" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5749,7 +5804,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.05" customHeight="1">
+    <row r="2" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -5798,7 +5853,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.05" customHeight="1">
+    <row r="3" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -5847,7 +5902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.05" customHeight="1">
+    <row r="4" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -5896,7 +5951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.05" customHeight="1">
+    <row r="5" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -5945,7 +6000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.05" customHeight="1">
+    <row r="6" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -5994,7 +6049,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.05" customHeight="1">
+    <row r="7" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -6043,7 +6098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.05" customHeight="1">
+    <row r="8" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -6092,7 +6147,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17.05" customHeight="1">
+    <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -6141,7 +6196,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="23"/>
       <c r="C10" s="2"/>
@@ -6160,7 +6215,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="23"/>
       <c r="C11" s="2"/>
@@ -6179,7 +6234,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="23"/>
       <c r="C12" s="2"/>
@@ -6198,7 +6253,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="23"/>
       <c r="C13" s="2"/>
@@ -6217,7 +6272,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="18" t="s">
         <v>159</v>
@@ -6238,7 +6293,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="18"/>
       <c r="C15" s="2"/>
@@ -6257,7 +6312,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="18" t="s">
         <v>160</v>
@@ -6280,7 +6335,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1">
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="1" t="s">
@@ -6301,7 +6356,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1">
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="1" t="s">
@@ -6322,7 +6377,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="23"/>
       <c r="C19" s="2"/>
@@ -6341,7 +6396,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1">
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="18" t="s">
         <v>164</v>
@@ -6374,25 +6429,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="11" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" customWidth="1"/>
     <col min="13" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="19.265625" customWidth="1"/>
-    <col min="16" max="16" width="190.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.9296875" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="190.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5" customHeight="1">
+    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -6440,7 +6497,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -6459,30 +6516,36 @@
       <c r="F2" s="2">
         <v>90</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="G2" s="2">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>129</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>131</v>
+        <v>240</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>133</v>
+        <v>242</v>
       </c>
       <c r="Q2" s="2">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -6501,30 +6564,36 @@
       <c r="F3" s="2">
         <v>90</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="G3" s="2">
+        <v>33</v>
+      </c>
+      <c r="H3" s="2">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="K3" s="1" t="s">
-        <v>129</v>
+        <v>244</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>134</v>
+        <v>243</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="1" t="s">
-        <v>132</v>
+        <v>247</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>136</v>
+        <v>246</v>
       </c>
       <c r="Q3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -6572,7 +6641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -6620,7 +6689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -6668,7 +6737,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -6716,7 +6785,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -6764,7 +6833,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1">
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -6812,7 +6881,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6822,6 +6891,84 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="18"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="23"/>
+      <c r="C16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="23"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="23"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="29" t="s">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6833,19 +6980,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -6874,7 +7023,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -6893,7 +7042,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -6912,7 +7061,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -6935,7 +7084,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -6958,7 +7107,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -6981,7 +7130,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>202</v>
       </c>
@@ -7004,29 +7153,53 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2">
+        <v>60</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2">
+        <v>65</v>
+      </c>
+      <c r="F9" s="2">
+        <v>40</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -7047,17 +7220,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="10.86328125" customWidth="1"/>
+    <col min="1" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" customHeight="1">
+    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>28</v>
       </c>
@@ -7086,7 +7259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -7097,7 +7270,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -7108,7 +7281,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -7119,7 +7292,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7130,7 +7303,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7141,7 +7314,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -7152,7 +7325,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -7163,7 +7336,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -7174,7 +7347,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -7195,22 +7368,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="28.19921875" customWidth="1"/>
-    <col min="3" max="3" width="49.46484375" customWidth="1"/>
-    <col min="4" max="256" width="10.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5" customWidth="1"/>
+    <col min="4" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.05" customHeight="1">
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -7223,7 +7396,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="34" customHeight="1">
+    <row r="2" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
@@ -7236,7 +7409,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="17.05" customHeight="1">
+    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -7249,7 +7422,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="17.05" customHeight="1">
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -7262,7 +7435,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="34" customHeight="1">
+    <row r="5" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -7275,7 +7448,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="17.05" customHeight="1">
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
@@ -7288,7 +7461,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="17.05" customHeight="1">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -7301,7 +7474,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1">
+    <row r="8" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -7314,7 +7487,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="34" customHeight="1">
+    <row r="9" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -7327,7 +7500,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="34" customHeight="1">
+    <row r="10" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -7340,7 +7513,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -7353,7 +7526,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="34" customHeight="1">
+    <row r="12" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
@@ -7366,7 +7539,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="51" customHeight="1">
+    <row r="13" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -7379,7 +7552,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="68.05" customHeight="1">
+    <row r="14" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>60</v>
       </c>
@@ -7392,7 +7565,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="34" customHeight="1">
+    <row r="15" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
@@ -7405,7 +7578,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="17.05" customHeight="1">
+    <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>64</v>
       </c>
@@ -7418,7 +7591,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="34" customHeight="1">
+    <row r="17" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
@@ -7431,7 +7604,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="17.05" customHeight="1">
+    <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -7444,7 +7617,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="17.05" customHeight="1">
+    <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>70</v>
       </c>
@@ -7457,7 +7630,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="17.05" customHeight="1">
+    <row r="20" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
@@ -7470,7 +7643,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="34" customHeight="1">
+    <row r="21" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>74</v>
       </c>
@@ -7483,7 +7656,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="34" customHeight="1">
+    <row r="22" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
@@ -7496,7 +7669,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="34" customHeight="1">
+    <row r="23" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>78</v>
       </c>
@@ -7509,7 +7682,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="34" customHeight="1">
+    <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -7522,7 +7695,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="51" customHeight="1">
+    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>82</v>
       </c>
@@ -7535,7 +7708,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="34" customHeight="1">
+    <row r="26" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>84</v>
       </c>
@@ -7548,7 +7721,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="136" customHeight="1">
+    <row r="27" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>86</v>
       </c>
@@ -7561,7 +7734,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="17.05" customHeight="1">
+    <row r="28" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>88</v>
       </c>
@@ -7574,7 +7747,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="34" customHeight="1">
+    <row r="29" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
@@ -7587,7 +7760,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="17.05" customHeight="1">
+    <row r="30" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
@@ -7600,7 +7773,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="17.05" customHeight="1">
+    <row r="31" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
         <v>94</v>
       </c>
@@ -7613,7 +7786,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="34" customHeight="1">
+    <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
         <v>96</v>
       </c>
@@ -7626,7 +7799,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="17.05" customHeight="1">
+    <row r="33" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>98</v>
       </c>
@@ -7639,7 +7812,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="34" customHeight="1">
+    <row r="34" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>202</v>
       </c>
@@ -7652,7 +7825,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="51" customHeight="1">
+    <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>205</v>
       </c>
@@ -7665,7 +7838,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="34" customHeight="1">
+    <row r="36" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>208</v>
       </c>
@@ -7678,7 +7851,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="34" customHeight="1">
+    <row r="37" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>211</v>
       </c>
@@ -7691,7 +7864,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="34" customHeight="1">
+    <row r="38" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
         <v>214</v>
       </c>
@@ -7704,7 +7877,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="34" customHeight="1">
+    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>217</v>
       </c>
@@ -7717,7 +7890,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="34" customHeight="1">
+    <row r="40" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
         <v>220</v>
       </c>
@@ -7730,7 +7903,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="34" customHeight="1">
+    <row r="41" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>223</v>
       </c>
@@ -7743,7 +7916,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" ht="34" customHeight="1">
+    <row r="42" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
         <v>226</v>
       </c>
@@ -7756,7 +7929,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="34" customHeight="1">
+    <row r="43" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Updated xlsx sheet with Sprint03 details
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/Java/Final Pro/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens\Courses\CS-555-Agile Methods for SW Eng\GEDCOM_Project\CS_555_JAVS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FAE56A-2210-493C-984D-CFD118E5F659}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,13 +23,10 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +34,15 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="263">
   <si>
     <t>Initials</t>
   </si>
@@ -800,18 +801,48 @@
   </si>
   <si>
     <t>Late start of new things to be implemented</t>
+  </si>
+  <si>
+    <t>US_CheckUniqueness.java</t>
+  </si>
+  <si>
+    <t>findDuplicateSpousedetails</t>
+  </si>
+  <si>
+    <t>10-39</t>
+  </si>
+  <si>
+    <t>Test_US24UniqueFamilyBySpouse</t>
+  </si>
+  <si>
+    <t>Test_US09BirthAfterDeathOfParents</t>
+  </si>
+  <si>
+    <t>testUniqueFamilyBySpouseRefactoredError, testUniqueFamilyBySpouseRefactoredSuccess</t>
+  </si>
+  <si>
+    <t>US_DatesCheckInFamily</t>
+  </si>
+  <si>
+    <t>findBirthBeforeDeathOfParents</t>
+  </si>
+  <si>
+    <t>250-285</t>
+  </si>
+  <si>
+    <t>testBirthAfterDeathOfMother,testBirthAfterDeathOfFather,testBirthAfterDeathOfMotherFather,testBirthBeforeDeathOfMotherFather,testBirthWhenMotherFatherAlive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
     <numFmt numFmtId="166" formatCode="m&quot;-&quot;yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -832,6 +863,25 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -962,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1009,6 +1059,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,7 +1199,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1108,10 +1212,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.095185"/>
-          <c:y val="0.0546885"/>
-          <c:w val="0.899815"/>
-          <c:h val="0.844287"/>
+          <c:x val="9.5185000000000006E-2"/>
+          <c:y val="5.4688500000000001E-2"/>
+          <c:w val="0.89981500000000003"/>
+          <c:h val="0.84428700000000001"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1154,16 +1258,16 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046.0</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42060.0</c:v>
+                  <c:v>42060</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42087.0</c:v>
+                  <c:v>42087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,25 +1279,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4D8D-48F0-9F2D-0F8AAA21AC8A}"/>
             </c:ext>
@@ -1342,7 +1446,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1355,10 +1459,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0738533"/>
-          <c:y val="0.0546885"/>
-          <c:w val="0.921147"/>
-          <c:h val="0.844287"/>
+          <c:x val="7.3853299999999997E-2"/>
+          <c:y val="5.4688500000000001E-2"/>
+          <c:w val="0.92114700000000005"/>
+          <c:h val="0.84428700000000001"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1404,13 +1508,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046.0</c:v>
+                  <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42059.0</c:v>
+                  <c:v>42059</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="m/d/yy">
-                  <c:v>42087.0</c:v>
+                <c:pt idx="2" formatCode="m/d/yyyy">
+                  <c:v>42087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1422,19 +1526,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2690-4E11-B0A0-7E616747BB0B}"/>
             </c:ext>
@@ -1543,8 +1647,8 @@
         <c:crossAx val="1013530416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="8.0"/>
-        <c:minorUnit val="4.0"/>
+        <c:majorUnit val="8"/>
+        <c:minorUnit val="4"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1602,7 +1706,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1742,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1657,7 +1761,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1760,7 +1864,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1782,7 +1886,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -1908,7 +2012,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1927,7 +2031,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2030,7 +2134,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2052,7 +2156,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2131,7 +2235,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2150,7 +2254,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2253,7 +2357,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2275,7 +2379,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2354,7 +2458,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2373,7 +2477,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2476,7 +2580,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2498,7 +2602,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2624,7 +2728,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2643,7 +2747,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2746,7 +2850,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2768,7 +2872,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2847,7 +2951,7 @@
         <xdr:cNvPr id="20" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2866,7 +2970,7 @@
           <xdr:cNvPr id="18" name="Shape 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2969,7 +3073,7 @@
           <xdr:cNvPr id="19" name="Shape 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2991,7 +3095,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3075,7 +3179,7 @@
         <xdr:cNvPr id="22" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4200,21 +4304,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4231,14 +4335,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -4255,7 +4359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -4272,7 +4376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -4289,7 +4393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4306,21 +4410,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4331,7 +4435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4348,24 +4452,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -4382,7 +4486,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4399,7 +4503,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4416,7 +4520,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4433,7 +4537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4450,7 +4554,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4467,7 +4571,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -4484,7 +4588,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -4501,7 +4605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4518,7 +4622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -4535,7 +4639,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -4552,7 +4656,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -4569,7 +4673,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -4586,7 +4690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -4599,7 +4703,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -4616,7 +4720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15" customHeight="1">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -4633,7 +4737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -4646,7 +4750,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -4663,7 +4767,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -4680,7 +4784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -4693,7 +4797,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -4706,7 +4810,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -4723,7 +4827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -4740,7 +4844,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -4753,7 +4857,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -4770,7 +4874,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -4783,7 +4887,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="2">
         <v>4</v>
       </c>
@@ -4796,7 +4900,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>4</v>
       </c>
@@ -4809,7 +4913,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -4822,7 +4926,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15" customHeight="1">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -4839,7 +4943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>4</v>
       </c>
@@ -4852,7 +4956,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15" customHeight="1">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -4869,7 +4973,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15" customHeight="1">
       <c r="A33" s="2">
         <v>4</v>
       </c>
@@ -4882,7 +4986,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="14.25" customHeight="1">
       <c r="A34" s="28">
         <v>3</v>
       </c>
@@ -4909,25 +5013,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.83203125" customWidth="1"/>
+    <col min="7" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="12.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4939,7 +5043,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="12.95" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -4951,7 +5055,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="12.95" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -4963,7 +5067,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="12.95" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4973,7 +5077,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="12.95" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
@@ -4985,7 +5089,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="12.95" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -4997,7 +5101,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="12.95" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5007,7 +5111,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="12.95" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -5019,7 +5123,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="12.95" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5029,7 +5133,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="12.95" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5039,7 +5143,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="12.95" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5049,7 +5153,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="12.95" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5059,7 +5163,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="12.95" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5069,7 +5173,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="12.95" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -5093,7 +5197,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="12.95" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -5111,7 +5215,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="12.95" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>113</v>
       </c>
@@ -5137,7 +5241,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="12.95" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
@@ -5163,7 +5267,7 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -5187,7 +5291,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="12.95" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
@@ -5211,7 +5315,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="13"/>
@@ -5221,7 +5325,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="12.95" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5231,7 +5335,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="12.95" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5241,7 +5345,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="12.95" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5251,7 +5355,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="12.95" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5261,7 +5365,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="12.95" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5271,7 +5375,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="12.95" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5281,7 +5385,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="12.95" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -5291,7 +5395,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="12.95" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -5301,7 +5405,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="12.95" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -5311,7 +5415,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="12.95" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5321,7 +5425,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="12.95" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -5331,7 +5435,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="12.95" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -5341,7 +5445,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="12.95" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -5351,7 +5455,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="12.95" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -5361,7 +5465,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="12.95" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -5371,7 +5475,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="12.95" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -5381,7 +5485,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="12.95" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -5391,7 +5495,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="12.95" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -5401,7 +5505,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="12.95" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -5422,25 +5526,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.83203125" customWidth="1"/>
+    <col min="7" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="12.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -5461,7 +5565,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="12.95" customHeight="1">
       <c r="A2" s="15">
         <v>42046</v>
       </c>
@@ -5476,7 +5580,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="12.95" customHeight="1">
       <c r="A3" s="15">
         <v>42059</v>
       </c>
@@ -5499,7 +5603,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="12.95" customHeight="1">
       <c r="A4" s="17">
         <v>42087</v>
       </c>
@@ -5518,7 +5622,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="12.95" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5527,7 +5631,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="12.95" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5536,7 +5640,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="12.95" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5545,7 +5649,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="12.95" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5554,7 +5658,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="12.95" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5563,7 +5667,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="12.95" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5572,7 +5676,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="12.95" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5581,7 +5685,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="12.95" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5590,7 +5694,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="12.95" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5599,7 +5703,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="12.95" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5608,7 +5712,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="12.95" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5617,7 +5721,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="12.95" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5626,7 +5730,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="12.95" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -5635,7 +5739,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="12.95" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5644,7 +5748,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="12.95" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -5653,7 +5757,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="12.95" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5662,7 +5766,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="12.95" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5671,7 +5775,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="12.95" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5680,7 +5784,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="12.95" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5689,7 +5793,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="12.95" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5698,7 +5802,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="12.95" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5707,7 +5811,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="12.95" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5727,35 +5831,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.375" customWidth="1"/>
+    <col min="4" max="4" width="8.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" customWidth="1"/>
+    <col min="14" max="14" width="1.875" customWidth="1"/>
+    <col min="15" max="15" width="10.125" customWidth="1"/>
     <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.125" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5804,7 +5908,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -5853,7 +5957,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -5902,7 +6006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -5951,7 +6055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -6000,7 +6104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -6049,7 +6153,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -6098,7 +6202,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -6147,7 +6251,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -6196,7 +6300,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="23"/>
       <c r="C10" s="2"/>
@@ -6215,7 +6319,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="23"/>
       <c r="C11" s="2"/>
@@ -6234,7 +6338,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="23"/>
       <c r="C12" s="2"/>
@@ -6253,7 +6357,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="23"/>
       <c r="C13" s="2"/>
@@ -6272,7 +6376,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="18" t="s">
         <v>159</v>
@@ -6293,7 +6397,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="18"/>
       <c r="C15" s="2"/>
@@ -6312,7 +6416,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="18" t="s">
         <v>160</v>
@@ -6335,7 +6439,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="1" t="s">
@@ -6356,7 +6460,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="1" t="s">
@@ -6377,7 +6481,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="23"/>
       <c r="C19" s="2"/>
@@ -6396,7 +6500,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="18" t="s">
         <v>164</v>
@@ -6429,27 +6533,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="K1" sqref="K1:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.625" customWidth="1"/>
     <col min="13" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="190.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.375" customWidth="1"/>
+    <col min="16" max="16" width="190.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -6497,7 +6601,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -6545,7 +6649,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -6593,7 +6697,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -6641,7 +6745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -6689,7 +6793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -6737,7 +6841,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -6785,7 +6889,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -6833,7 +6937,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -6881,7 +6985,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6892,7 +6996,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1">
       <c r="B13" s="18" t="s">
         <v>159</v>
       </c>
@@ -6902,7 +7006,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="14.25" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6910,7 +7014,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" ht="14.25" customHeight="1">
       <c r="B15" s="18" t="s">
         <v>160</v>
       </c>
@@ -6922,7 +7026,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="B16" s="23"/>
       <c r="C16" s="1" t="s">
         <v>249</v>
@@ -6932,7 +7036,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="14.25" customHeight="1">
       <c r="B17" s="23"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
@@ -6940,7 +7044,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="14.25" customHeight="1">
       <c r="B18" s="23"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -6948,7 +7052,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="14.25" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>164</v>
       </c>
@@ -6960,12 +7064,12 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="14.25" customHeight="1">
       <c r="C20" s="29" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="14.25" customHeight="1">
       <c r="C21" s="29" t="s">
         <v>251</v>
       </c>
@@ -6980,239 +7084,364 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="256" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" style="34" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="34" customWidth="1"/>
+    <col min="3" max="9" width="11" style="34" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="34" customWidth="1"/>
+    <col min="11" max="11" width="11" style="46" customWidth="1"/>
+    <col min="12" max="15" width="11" style="34" customWidth="1"/>
+    <col min="16" max="16" width="11" style="43" customWidth="1"/>
+    <col min="17" max="256" width="11" style="34" customWidth="1"/>
+    <col min="257" max="16384" width="11" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="25.5" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="33"/>
+      <c r="N1" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="O1" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1">
+      <c r="A2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="E2" s="33">
+        <v>50</v>
+      </c>
+      <c r="F2" s="33">
+        <v>50</v>
+      </c>
+      <c r="G2" s="33">
+        <v>35</v>
+      </c>
+      <c r="H2" s="33">
+        <v>30</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="M2" s="33"/>
+      <c r="N2" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="P2" s="42">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1">
+      <c r="A3" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+      <c r="E3" s="33">
+        <v>50</v>
+      </c>
+      <c r="F3" s="33">
+        <v>50</v>
+      </c>
+      <c r="G3" s="33">
+        <v>29</v>
+      </c>
+      <c r="H3" s="33">
+        <v>30</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="M3" s="33"/>
+      <c r="N3" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="P3" s="42">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1">
+      <c r="A4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="33">
         <v>70</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="33">
         <v>90</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="42"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1">
+      <c r="A5" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="33">
         <v>50</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="33">
         <v>60</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="42"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1">
+      <c r="A6" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="33">
         <v>50</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="33">
         <v>60</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="29" t="s">
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="42"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1">
+      <c r="A7" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="33">
         <v>50</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="33">
         <v>60</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="42"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1">
+      <c r="A8" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="33">
         <v>60</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="33">
         <v>45</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="42"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1">
+      <c r="A9" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="33">
         <v>65</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="33">
         <v>40</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="42"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -7220,17 +7449,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="10.83203125" customWidth="1"/>
+    <col min="1" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="27.95" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>28</v>
       </c>
@@ -7259,7 +7488,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -7270,7 +7499,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -7281,7 +7510,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -7292,7 +7521,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7303,7 +7532,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7314,7 +7543,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -7325,7 +7554,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -7336,7 +7565,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -7347,7 +7576,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -7368,22 +7597,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
     <col min="3" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="256" width="10.83203125" customWidth="1"/>
+    <col min="4" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="14.1" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -7396,7 +7625,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
@@ -7409,7 +7638,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -7422,7 +7651,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -7435,7 +7664,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -7448,7 +7677,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
@@ -7461,7 +7690,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -7474,7 +7703,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="51" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -7487,7 +7716,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -7500,7 +7729,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -7513,7 +7742,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -7526,7 +7755,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
@@ -7539,7 +7768,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="51" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -7552,7 +7781,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="68.099999999999994" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>60</v>
       </c>
@@ -7565,7 +7794,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
@@ -7578,7 +7807,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>64</v>
       </c>
@@ -7591,7 +7820,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
@@ -7604,7 +7833,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -7617,7 +7846,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>70</v>
       </c>
@@ -7630,7 +7859,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
@@ -7643,7 +7872,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>74</v>
       </c>
@@ -7656,7 +7885,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
@@ -7669,7 +7898,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>78</v>
       </c>
@@ -7682,7 +7911,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -7695,7 +7924,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="51" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>82</v>
       </c>
@@ -7708,7 +7937,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>84</v>
       </c>
@@ -7721,7 +7950,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="135.94999999999999" customHeight="1">
       <c r="A27" s="5" t="s">
         <v>86</v>
       </c>
@@ -7734,7 +7963,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>88</v>
       </c>
@@ -7747,7 +7976,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
@@ -7760,7 +7989,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
@@ -7773,7 +8002,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>94</v>
       </c>
@@ -7786,7 +8015,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>96</v>
       </c>
@@ -7799,7 +8028,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>98</v>
       </c>
@@ -7812,7 +8041,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>202</v>
       </c>
@@ -7825,7 +8054,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="51" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>205</v>
       </c>
@@ -7838,7 +8067,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>208</v>
       </c>
@@ -7851,7 +8080,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>211</v>
       </c>
@@ -7864,7 +8093,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>214</v>
       </c>
@@ -7877,7 +8106,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>217</v>
       </c>
@@ -7890,7 +8119,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>220</v>
       </c>
@@ -7903,7 +8132,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>223</v>
       </c>
@@ -7916,7 +8145,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>226</v>
       </c>
@@ -7929,7 +8158,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
updated spreadsheet for US 31 and 33
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens\Courses\CS-555-Agile Methods for SW Eng\GEDCOM_Project\CS_555_JAVS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FAE56A-2210-493C-984D-CFD118E5F659}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACD93DA-40A8-432B-8FBB-7334F5DE9A7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="264">
   <si>
     <t>Initials</t>
   </si>
@@ -831,6 +831,9 @@
   </si>
   <si>
     <t>testBirthAfterDeathOfMother,testBirthAfterDeathOfFather,testBirthAfterDeathOfMotherFather,testBirthBeforeDeathOfMotherFather,testBirthWhenMotherFatherAlive</t>
+  </si>
+  <si>
+    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -1886,7 +1889,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2156,7 +2159,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2379,7 +2382,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2602,7 +2605,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2872,7 +2875,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3095,7 +3098,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -4455,7 +4458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
@@ -7087,8 +7090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
@@ -7319,7 +7322,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="E6" s="33">
         <v>50</v>
@@ -7327,9 +7330,15 @@
       <c r="F6" s="33">
         <v>60</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
+      <c r="G6" s="33">
+        <v>23</v>
+      </c>
+      <c r="H6" s="33">
+        <v>60</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>166</v>
+      </c>
       <c r="J6" s="35"/>
       <c r="K6" s="45"/>
       <c r="L6" s="35"/>
@@ -7349,7 +7358,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="E7" s="33">
         <v>50</v>
@@ -7357,9 +7366,15 @@
       <c r="F7" s="33">
         <v>60</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
+      <c r="G7" s="33">
+        <v>14</v>
+      </c>
+      <c r="H7" s="33">
+        <v>20</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>166</v>
+      </c>
       <c r="J7" s="35"/>
       <c r="K7" s="45"/>
       <c r="L7" s="35"/>
@@ -7600,8 +7615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>

</xml_diff>

<commit_message>
Added user story US27 and US30
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/Java/Final Pro/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACD93DA-40A8-432B-8FBB-7334F5DE9A7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +22,13 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,15 +36,12 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="263">
   <si>
     <t>Initials</t>
   </si>
@@ -831,21 +830,18 @@
   </si>
   <si>
     <t>testBirthAfterDeathOfMother,testBirthAfterDeathOfFather,testBirthAfterDeathOfMotherFather,testBirthBeforeDeathOfMotherFather,testBirthWhenMotherFatherAlive</t>
-  </si>
-  <si>
-    <t>testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
     <numFmt numFmtId="166" formatCode="m&quot;-&quot;yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1202,7 +1198,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1215,10 +1211,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5185000000000006E-2"/>
-          <c:y val="5.4688500000000001E-2"/>
-          <c:w val="0.89981500000000003"/>
-          <c:h val="0.84428700000000001"/>
+          <c:x val="0.095185"/>
+          <c:y val="0.0546885"/>
+          <c:w val="0.899815"/>
+          <c:h val="0.844287"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1261,16 +1257,16 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42060</c:v>
+                  <c:v>42060.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42087</c:v>
+                  <c:v>42087.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,25 +1278,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4D8D-48F0-9F2D-0F8AAA21AC8A}"/>
             </c:ext>
@@ -1316,11 +1312,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1041759056"/>
-        <c:axId val="1041746144"/>
+        <c:axId val="1856930864"/>
+        <c:axId val="1856932912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1041759056"/>
+        <c:axId val="1856930864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1354,14 +1350,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1041746144"/>
+        <c:crossAx val="1856932912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1041746144"/>
+        <c:axId val="1856932912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1041759056"/>
+        <c:crossAx val="1856930864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1449,7 +1445,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1462,10 +1458,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.3853299999999997E-2"/>
-          <c:y val="5.4688500000000001E-2"/>
-          <c:w val="0.92114700000000005"/>
-          <c:h val="0.84428700000000001"/>
+          <c:x val="0.0738533"/>
+          <c:y val="0.0546885"/>
+          <c:w val="0.921147"/>
+          <c:h val="0.844287"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1511,13 +1507,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42059</c:v>
+                  <c:v>42059.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="m/d/yyyy">
-                  <c:v>42087</c:v>
+                <c:pt idx="2" formatCode="m/d/yy">
+                  <c:v>42087.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1529,19 +1525,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2690-4E11-B0A0-7E616747BB0B}"/>
             </c:ext>
@@ -1557,11 +1553,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1013530416"/>
-        <c:axId val="1013895728"/>
+        <c:axId val="1859481920"/>
+        <c:axId val="1859483552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1013530416"/>
+        <c:axId val="1859481920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,14 +1591,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1013895728"/>
+        <c:crossAx val="1859483552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1013895728"/>
+        <c:axId val="1859483552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,11 +1643,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1013530416"/>
+        <c:crossAx val="1859481920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="8"/>
-        <c:minorUnit val="4"/>
+        <c:majorUnit val="8.0"/>
+        <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1709,7 +1705,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1745,7 +1741,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1764,7 +1760,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1867,7 +1863,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1889,7 +1885,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2015,7 +2011,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2034,7 +2030,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2137,7 +2133,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2159,7 +2155,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2238,7 +2234,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2257,7 +2253,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2360,7 +2356,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2382,7 +2378,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2461,7 +2457,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2480,7 +2476,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2583,7 +2579,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2605,7 +2601,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2731,7 +2727,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2750,7 +2746,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2853,7 +2849,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2875,7 +2871,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2954,7 +2950,7 @@
         <xdr:cNvPr id="20" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2973,7 +2969,7 @@
           <xdr:cNvPr id="18" name="Shape 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000012000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3076,7 +3072,7 @@
           <xdr:cNvPr id="19" name="Shape 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000013000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3098,7 +3094,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3182,7 +3178,7 @@
         <xdr:cNvPr id="22" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4307,21 +4303,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4338,14 +4334,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -4362,7 +4358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -4379,7 +4375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -4396,7 +4392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4413,21 +4409,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4438,7 +4434,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4455,24 +4451,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:D34"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="25.375" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -4489,7 +4485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4506,7 +4502,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4523,7 +4519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4540,7 +4536,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4557,7 +4553,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4574,7 +4570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -4591,7 +4587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -4608,7 +4604,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4625,7 +4621,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -4642,7 +4638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -4659,7 +4655,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -4676,7 +4672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -4693,7 +4689,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -4706,7 +4702,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -4723,7 +4719,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -4740,7 +4736,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -4753,7 +4749,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -4770,7 +4766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -4787,7 +4783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -4800,7 +4796,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -4813,7 +4809,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -4830,7 +4826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -4847,7 +4843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -4860,7 +4856,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -4877,7 +4873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -4890,7 +4886,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>4</v>
       </c>
@@ -4903,9 +4899,9 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>88</v>
@@ -4913,10 +4909,14 @@
       <c r="C28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="D28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -4929,7 +4929,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -4946,9 +4946,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>94</v>
@@ -4956,10 +4956,14 @@
       <c r="C31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1">
+      <c r="D31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -4976,7 +4980,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>4</v>
       </c>
@@ -4989,7 +4993,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1">
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="28">
         <v>3</v>
       </c>
@@ -5016,25 +5020,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.875" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.95" customHeight="1">
+    <row r="1" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -5046,7 +5050,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="12.95" customHeight="1">
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -5058,7 +5062,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="12.95" customHeight="1">
+    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -5070,7 +5074,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="12.95" customHeight="1">
+    <row r="4" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5080,7 +5084,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="12.95" customHeight="1">
+    <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
@@ -5092,7 +5096,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="12.95" customHeight="1">
+    <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -5104,7 +5108,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="12.95" customHeight="1">
+    <row r="7" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5114,7 +5118,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="12.95" customHeight="1">
+    <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -5126,7 +5130,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="12.95" customHeight="1">
+    <row r="9" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5136,7 +5140,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="12.95" customHeight="1">
+    <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5146,7 +5150,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="12.95" customHeight="1">
+    <row r="11" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5156,7 +5160,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="12.95" customHeight="1">
+    <row r="12" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5166,7 +5170,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="12.95" customHeight="1">
+    <row r="13" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5176,7 +5180,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="12.95" customHeight="1">
+    <row r="14" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -5200,7 +5204,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="12.95" customHeight="1">
+    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -5218,7 +5222,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="12.95" customHeight="1">
+    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>113</v>
       </c>
@@ -5244,7 +5248,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="12.95" customHeight="1">
+    <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
@@ -5270,7 +5274,7 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="12.95" customHeight="1">
+    <row r="18" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -5294,7 +5298,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="12.95" customHeight="1">
+    <row r="19" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
@@ -5318,7 +5322,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="12.95" customHeight="1">
+    <row r="20" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="13"/>
@@ -5328,7 +5332,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.95" customHeight="1">
+    <row r="21" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5338,7 +5342,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.95" customHeight="1">
+    <row r="22" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5348,7 +5352,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="12.95" customHeight="1">
+    <row r="23" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5358,7 +5362,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="12.95" customHeight="1">
+    <row r="24" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5368,7 +5372,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="12.95" customHeight="1">
+    <row r="25" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5378,7 +5382,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="12.95" customHeight="1">
+    <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5388,7 +5392,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="12.95" customHeight="1">
+    <row r="27" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -5398,7 +5402,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="12.95" customHeight="1">
+    <row r="28" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -5408,7 +5412,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="12.95" customHeight="1">
+    <row r="29" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -5418,7 +5422,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="12.95" customHeight="1">
+    <row r="30" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5428,7 +5432,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="12.95" customHeight="1">
+    <row r="31" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -5438,7 +5442,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="12.95" customHeight="1">
+    <row r="32" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -5448,7 +5452,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="12.95" customHeight="1">
+    <row r="33" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -5458,7 +5462,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="12.95" customHeight="1">
+    <row r="34" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -5468,7 +5472,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="12.95" customHeight="1">
+    <row r="35" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -5478,7 +5482,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="12.95" customHeight="1">
+    <row r="36" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -5488,7 +5492,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="12.95" customHeight="1">
+    <row r="37" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -5498,7 +5502,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="12.95" customHeight="1">
+    <row r="38" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -5508,7 +5512,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="12.95" customHeight="1">
+    <row r="39" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -5529,25 +5533,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.875" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.95" customHeight="1">
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -5568,7 +5572,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="12.95" customHeight="1">
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15">
         <v>42046</v>
       </c>
@@ -5583,7 +5587,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="12.95" customHeight="1">
+    <row r="3" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15">
         <v>42059</v>
       </c>
@@ -5606,7 +5610,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="12.95" customHeight="1">
+    <row r="4" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>42087</v>
       </c>
@@ -5625,7 +5629,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="12.95" customHeight="1">
+    <row r="5" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5634,7 +5638,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="12.95" customHeight="1">
+    <row r="6" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5643,7 +5647,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="12.95" customHeight="1">
+    <row r="7" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5652,7 +5656,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="12.95" customHeight="1">
+    <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5661,7 +5665,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="12.95" customHeight="1">
+    <row r="9" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5670,7 +5674,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="12.95" customHeight="1">
+    <row r="10" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5679,7 +5683,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="12.95" customHeight="1">
+    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5688,7 +5692,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="12.95" customHeight="1">
+    <row r="12" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5697,7 +5701,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="12.95" customHeight="1">
+    <row r="13" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5706,7 +5710,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="12.95" customHeight="1">
+    <row r="14" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5715,7 +5719,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="12.95" customHeight="1">
+    <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5724,7 +5728,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="12.95" customHeight="1">
+    <row r="16" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5733,7 +5737,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="12.95" customHeight="1">
+    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -5742,7 +5746,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="12.95" customHeight="1">
+    <row r="18" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5751,7 +5755,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="12.95" customHeight="1">
+    <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -5760,7 +5764,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="12.95" customHeight="1">
+    <row r="20" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5769,7 +5773,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="12.95" customHeight="1">
+    <row r="21" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5778,7 +5782,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="12.95" customHeight="1">
+    <row r="22" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5787,7 +5791,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="12.95" customHeight="1">
+    <row r="23" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5796,7 +5800,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="12.95" customHeight="1">
+    <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5805,7 +5809,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="12.95" customHeight="1">
+    <row r="25" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5814,7 +5818,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="12.95" customHeight="1">
+    <row r="26" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5834,35 +5838,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="7.375" customWidth="1"/>
-    <col min="4" max="4" width="8.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="19.125" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.875" customWidth="1"/>
-    <col min="15" max="15" width="10.125" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" customWidth="1"/>
     <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="10.125" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5911,7 +5915,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -5960,7 +5964,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -6009,7 +6013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -6058,7 +6062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -6107,7 +6111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -6156,7 +6160,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -6205,7 +6209,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -6254,7 +6258,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -6303,7 +6307,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="23"/>
       <c r="C10" s="2"/>
@@ -6322,7 +6326,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="23"/>
       <c r="C11" s="2"/>
@@ -6341,7 +6345,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="23"/>
       <c r="C12" s="2"/>
@@ -6360,7 +6364,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="23"/>
       <c r="C13" s="2"/>
@@ -6379,7 +6383,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="18" t="s">
         <v>159</v>
@@ -6400,7 +6404,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="18"/>
       <c r="C15" s="2"/>
@@ -6419,7 +6423,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="18" t="s">
         <v>160</v>
@@ -6442,7 +6446,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1">
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="1" t="s">
@@ -6463,7 +6467,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1">
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="1" t="s">
@@ -6484,7 +6488,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="23"/>
       <c r="C19" s="2"/>
@@ -6503,7 +6507,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1">
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="18" t="s">
         <v>164</v>
@@ -6536,27 +6540,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="22.625" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
     <col min="13" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="19.375" customWidth="1"/>
-    <col min="16" max="16" width="190.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="190.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5" customHeight="1">
+    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -6604,7 +6608,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -6652,7 +6656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -6700,7 +6704,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -6748,7 +6752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -6796,7 +6800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -6844,7 +6848,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -6892,7 +6896,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -6940,7 +6944,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1">
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -6988,7 +6992,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6999,7 +7003,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="14.25" customHeight="1">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="18" t="s">
         <v>159</v>
       </c>
@@ -7009,7 +7013,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="14.25" customHeight="1">
+    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="18"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -7017,7 +7021,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1">
+    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="18" t="s">
         <v>160</v>
       </c>
@@ -7029,7 +7033,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" customHeight="1">
+    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="23"/>
       <c r="C16" s="1" t="s">
         <v>249</v>
@@ -7039,7 +7043,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" ht="14.25" customHeight="1">
+    <row r="17" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="23"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
@@ -7047,7 +7051,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" ht="14.25" customHeight="1">
+    <row r="18" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="23"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -7055,7 +7059,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="14.25" customHeight="1">
+    <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
         <v>164</v>
       </c>
@@ -7067,12 +7071,12 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="14.25" customHeight="1">
+    <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C20" s="29" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="14.25" customHeight="1">
+    <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C21" s="29" t="s">
         <v>251</v>
       </c>
@@ -7087,17 +7091,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="34" customWidth="1"/>
-    <col min="2" max="2" width="22.625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="34" customWidth="1"/>
     <col min="3" max="9" width="11" style="34" customWidth="1"/>
     <col min="10" max="10" width="20.5" style="34" customWidth="1"/>
     <col min="11" max="11" width="11" style="46" customWidth="1"/>
@@ -7107,7 +7111,7 @@
     <col min="257" max="16384" width="11" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.5" customHeight="1">
+    <row r="1" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="30" t="s">
         <v>28</v>
       </c>
@@ -7155,7 +7159,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
         <v>55</v>
       </c>
@@ -7203,7 +7207,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="35" t="s">
         <v>82</v>
       </c>
@@ -7251,7 +7255,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="35" t="s">
         <v>62</v>
       </c>
@@ -7281,7 +7285,7 @@
       <c r="O4" s="36"/>
       <c r="P4" s="42"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="35" t="s">
         <v>52</v>
       </c>
@@ -7311,7 +7315,7 @@
       <c r="O5" s="36"/>
       <c r="P5" s="42"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="35" t="s">
         <v>96</v>
       </c>
@@ -7322,7 +7326,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>263</v>
+        <v>54</v>
       </c>
       <c r="E6" s="33">
         <v>50</v>
@@ -7330,15 +7334,9 @@
       <c r="F6" s="33">
         <v>60</v>
       </c>
-      <c r="G6" s="33">
-        <v>23</v>
-      </c>
-      <c r="H6" s="33">
-        <v>60</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>166</v>
-      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
       <c r="J6" s="35"/>
       <c r="K6" s="45"/>
       <c r="L6" s="35"/>
@@ -7347,7 +7345,7 @@
       <c r="O6" s="36"/>
       <c r="P6" s="42"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>202</v>
       </c>
@@ -7358,7 +7356,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>263</v>
+        <v>54</v>
       </c>
       <c r="E7" s="33">
         <v>50</v>
@@ -7366,15 +7364,9 @@
       <c r="F7" s="33">
         <v>60</v>
       </c>
-      <c r="G7" s="33">
-        <v>14</v>
-      </c>
-      <c r="H7" s="33">
-        <v>20</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>166</v>
-      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="35"/>
       <c r="K7" s="45"/>
       <c r="L7" s="35"/>
@@ -7383,7 +7375,7 @@
       <c r="O7" s="36"/>
       <c r="P7" s="42"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>88</v>
       </c>
@@ -7413,7 +7405,7 @@
       <c r="O8" s="36"/>
       <c r="P8" s="42"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>92</v>
       </c>
@@ -7443,7 +7435,7 @@
       <c r="O9" s="36"/>
       <c r="P9" s="42"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -7464,17 +7456,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="10.875" customWidth="1"/>
+    <col min="1" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95" customHeight="1">
+    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>28</v>
       </c>
@@ -7503,7 +7495,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -7514,7 +7506,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -7525,7 +7517,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -7536,7 +7528,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7547,7 +7539,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7558,7 +7550,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -7569,7 +7561,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -7580,7 +7572,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -7591,7 +7583,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -7612,22 +7604,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="256" width="10.875" customWidth="1"/>
+    <col min="4" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.1" customHeight="1">
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
@@ -7640,7 +7632,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="2" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
@@ -7653,7 +7645,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -7666,7 +7658,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -7679,7 +7671,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="5" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -7692,7 +7684,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
@@ -7705,7 +7697,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -7718,7 +7710,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1">
+    <row r="8" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -7731,7 +7723,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="9" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -7744,7 +7736,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="10" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -7757,7 +7749,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="11" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -7770,7 +7762,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="12" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
@@ -7783,7 +7775,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="51" customHeight="1">
+    <row r="13" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -7796,7 +7788,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="68.099999999999994" customHeight="1">
+    <row r="14" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>60</v>
       </c>
@@ -7809,7 +7801,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="15" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
@@ -7822,7 +7814,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>64</v>
       </c>
@@ -7835,7 +7827,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="17" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
@@ -7848,7 +7840,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -7861,7 +7853,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>70</v>
       </c>
@@ -7874,7 +7866,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
@@ -7887,7 +7879,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="21" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>74</v>
       </c>
@@ -7900,7 +7892,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="22" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
@@ -7913,7 +7905,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="23" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>78</v>
       </c>
@@ -7926,7 +7918,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -7939,7 +7931,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="51" customHeight="1">
+    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>82</v>
       </c>
@@ -7952,7 +7944,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="26" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>84</v>
       </c>
@@ -7965,7 +7957,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="135.94999999999999" customHeight="1">
+    <row r="27" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>86</v>
       </c>
@@ -7978,7 +7970,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>88</v>
       </c>
@@ -7991,7 +7983,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="29" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
@@ -8004,7 +7996,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
@@ -8017,7 +8009,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
         <v>94</v>
       </c>
@@ -8030,7 +8022,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
         <v>96</v>
       </c>
@@ -8043,7 +8035,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>98</v>
       </c>
@@ -8056,7 +8048,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="34" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>202</v>
       </c>
@@ -8069,7 +8061,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="51" customHeight="1">
+    <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>205</v>
       </c>
@@ -8082,7 +8074,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="36" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>208</v>
       </c>
@@ -8095,7 +8087,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="37" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>211</v>
       </c>
@@ -8108,7 +8100,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="38" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
         <v>214</v>
       </c>
@@ -8121,7 +8113,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>217</v>
       </c>
@@ -8134,7 +8126,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="40" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
         <v>220</v>
       </c>
@@ -8147,7 +8139,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="41" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>223</v>
       </c>
@@ -8160,7 +8152,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="42" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
         <v>226</v>
       </c>
@@ -8173,7 +8165,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="43" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Added All_Lists file - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1011,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1056,7 +1056,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4454,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4965,7 +4964,7 @@
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>96</v>
@@ -4994,10 +4993,10 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="28">
+      <c r="A34" s="2">
         <v>3</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="28" t="s">
         <v>202</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -6544,7 +6543,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7072,12 +7071,12 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>251</v>
       </c>
     </row>
@@ -7094,357 +7093,357 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11" style="34" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="34" customWidth="1"/>
-    <col min="3" max="9" width="11" style="34" customWidth="1"/>
-    <col min="10" max="10" width="20.5" style="34" customWidth="1"/>
-    <col min="11" max="11" width="11" style="46" customWidth="1"/>
-    <col min="12" max="15" width="11" style="34" customWidth="1"/>
-    <col min="16" max="16" width="11" style="43" customWidth="1"/>
-    <col min="17" max="256" width="11" style="34" customWidth="1"/>
-    <col min="257" max="16384" width="11" style="34"/>
+    <col min="1" max="1" width="11" style="33" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
+    <col min="3" max="9" width="11" style="33" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="33" customWidth="1"/>
+    <col min="11" max="11" width="11" style="45" customWidth="1"/>
+    <col min="12" max="15" width="11" style="33" customWidth="1"/>
+    <col min="16" max="16" width="11" style="42" customWidth="1"/>
+    <col min="17" max="256" width="11" style="33" customWidth="1"/>
+    <col min="257" max="16384" width="11" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="32" t="s">
+      <c r="M1" s="32"/>
+      <c r="N1" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="40" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <v>50</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="32">
         <v>50</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="32">
         <v>35</v>
       </c>
-      <c r="H2" s="33">
+      <c r="H2" s="32">
         <v>30</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="39" t="s">
         <v>260</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="40" t="s">
+      <c r="M2" s="32"/>
+      <c r="N2" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="P2" s="42">
+      <c r="P2" s="41">
         <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>50</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>50</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="32">
         <v>29</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="32">
         <v>30</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="40" t="s">
+      <c r="M3" s="32"/>
+      <c r="N3" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="P3" s="42">
+      <c r="P3" s="41">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>70</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>90</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="42"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="41"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>50</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>60</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="42"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="41"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="32">
         <v>50</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <v>60</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="42"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="41"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>50</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>60</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="42"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="41"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>60</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>45</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="42"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="41"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>65</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>40</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="42"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="41"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7607,8 +7606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updated all files - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="262">
   <si>
     <t>Initials</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Parents not too old</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>US13</t>
@@ -4453,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4689,14 +4686,12 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -4706,10 +4701,10 @@
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -4723,10 +4718,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -4740,10 +4735,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -4753,10 +4748,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -4770,10 +4765,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
@@ -4787,10 +4782,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -4800,10 +4795,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -4813,10 +4808,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
@@ -4830,10 +4825,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>20</v>
@@ -4847,10 +4842,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -4860,10 +4855,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>5</v>
@@ -4877,10 +4872,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -4890,10 +4885,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -4903,10 +4898,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>20</v>
@@ -4920,10 +4915,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -4933,10 +4928,10 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>15</v>
@@ -4950,10 +4945,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>20</v>
@@ -4967,10 +4962,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
@@ -4984,10 +4979,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -4997,10 +4992,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -5039,7 +5034,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5051,7 +5046,7 @@
     </row>
     <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5063,7 +5058,7 @@
     </row>
     <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -5085,7 +5080,7 @@
     </row>
     <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5097,7 +5092,7 @@
     </row>
     <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5119,7 +5114,7 @@
     </row>
     <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5184,28 +5179,28 @@
         <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="8">
         <v>42046</v>
@@ -5223,7 +5218,7 @@
     </row>
     <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="8">
         <v>42060</v>
@@ -5249,7 +5244,7 @@
     </row>
     <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="8">
         <v>42087</v>
@@ -5275,7 +5270,7 @@
     </row>
     <row r="18" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9">
@@ -5299,7 +5294,7 @@
     </row>
     <row r="19" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="9">
@@ -5552,22 +5547,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G1" s="4"/>
     </row>
@@ -5879,39 +5874,39 @@
         <v>31</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>34</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -5925,7 +5920,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2">
         <v>100</v>
@@ -5940,24 +5935,24 @@
         <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="Q2" s="2">
         <v>113</v>
@@ -5974,7 +5969,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
@@ -5989,24 +5984,24 @@
         <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L3" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q3" s="2">
         <v>20</v>
@@ -6023,7 +6018,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="2">
         <v>102</v>
@@ -6038,24 +6033,24 @@
         <v>100</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>137</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>138</v>
       </c>
       <c r="M4" s="22">
         <v>48944</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="P4" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="P4" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="Q4" s="2">
         <v>8</v>
@@ -6072,7 +6067,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
@@ -6087,24 +6082,24 @@
         <v>50</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q5" s="2">
         <v>11</v>
@@ -6121,7 +6116,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2">
         <v>90</v>
@@ -6136,24 +6131,24 @@
         <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="M6" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P6" s="21" t="s">
         <v>147</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>148</v>
       </c>
       <c r="Q6" s="2">
         <v>232</v>
@@ -6170,7 +6165,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="2">
         <v>100</v>
@@ -6185,24 +6180,24 @@
         <v>180</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L7" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="2">
         <v>43</v>
@@ -6219,7 +6214,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="2">
         <v>105</v>
@@ -6234,24 +6229,24 @@
         <v>75</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M8" s="22">
         <v>51470</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P8" s="21" t="s">
         <v>153</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>154</v>
       </c>
       <c r="Q8" s="2">
         <v>182</v>
@@ -6268,7 +6263,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="2">
         <v>100</v>
@@ -6283,24 +6278,24 @@
         <v>60</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L9" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P9" s="21" t="s">
         <v>157</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>158</v>
       </c>
       <c r="Q9" s="2">
         <v>167</v>
@@ -6385,7 +6380,7 @@
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6425,10 +6420,10 @@
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -6449,7 +6444,7 @@
       <c r="A17" s="2"/>
       <c r="B17" s="23"/>
       <c r="C17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -6470,7 +6465,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="23"/>
       <c r="C18" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -6509,10 +6504,10 @@
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -6573,46 +6568,46 @@
         <v>31</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K1" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -6633,23 +6628,23 @@
         <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L2" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="Q2" s="2">
         <v>85</v>
@@ -6657,10 +6652,10 @@
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -6681,23 +6676,23 @@
         <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q3" s="2">
         <v>68</v>
@@ -6705,10 +6700,10 @@
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -6729,23 +6724,23 @@
         <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>137</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>138</v>
       </c>
       <c r="M4" s="22">
         <v>48944</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="P4" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="P4" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="Q4" s="2">
         <v>8</v>
@@ -6777,23 +6772,23 @@
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q5" s="2">
         <v>11</v>
@@ -6801,10 +6796,10 @@
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -6825,23 +6820,23 @@
         <v>20</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q6" s="2">
         <v>232</v>
@@ -6849,10 +6844,10 @@
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -6873,23 +6868,23 @@
         <v>10</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L7" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q7" s="2">
         <v>43</v>
@@ -6897,10 +6892,10 @@
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -6921,23 +6916,23 @@
         <v>90</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M8" s="22">
         <v>51470</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P8" s="21" t="s">
         <v>153</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>154</v>
       </c>
       <c r="Q8" s="2">
         <v>182</v>
@@ -6969,23 +6964,23 @@
         <v>90</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L9" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P9" s="21" t="s">
         <v>157</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>158</v>
       </c>
       <c r="Q9" s="2">
         <v>167</v>
@@ -7004,7 +6999,7 @@
     </row>
     <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -7022,10 +7017,10 @@
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -7035,7 +7030,7 @@
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="23"/>
       <c r="C16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -7060,10 +7055,10 @@
     </row>
     <row r="19" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -7072,12 +7067,12 @@
     </row>
     <row r="20" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C20" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C21" s="28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -7124,38 +7119,38 @@
         <v>31</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="30" t="s">
         <v>34</v>
       </c>
       <c r="J1" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="L1" s="31" t="s">
         <v>122</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>123</v>
       </c>
       <c r="M1" s="32"/>
       <c r="N1" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="40" t="s">
         <v>125</v>
-      </c>
-      <c r="P1" s="40" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7166,7 +7161,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>54</v>
@@ -7184,23 +7179,23 @@
         <v>30</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J2" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="K2" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="L2" s="39" t="s">
         <v>260</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>261</v>
       </c>
       <c r="M2" s="32"/>
       <c r="N2" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P2" s="41">
         <v>236</v>
@@ -7208,13 +7203,13 @@
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>83</v>
-      </c>
       <c r="C3" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>54</v>
@@ -7232,23 +7227,23 @@
         <v>30</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J3" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="L3" s="39" t="s">
         <v>254</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="M3" s="32"/>
       <c r="N3" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O3" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P3" s="41">
         <v>96</v>
@@ -7256,13 +7251,13 @@
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>63</v>
-      </c>
       <c r="C4" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>54</v>
@@ -7292,7 +7287,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>54</v>
@@ -7316,10 +7311,10 @@
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>97</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>15</v>
@@ -7346,10 +7341,10 @@
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>202</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>203</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>15</v>
@@ -7376,10 +7371,10 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>20</v>
@@ -7406,10 +7401,10 @@
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>20</v>
@@ -7479,16 +7474,16 @@
         <v>31</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="I1" s="25" t="s">
         <v>34</v>
@@ -7626,7 +7621,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -7639,7 +7634,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -7652,7 +7647,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -7665,7 +7660,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -7678,7 +7673,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -7691,7 +7686,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7704,7 +7699,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -7717,7 +7712,7 @@
         <v>38</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -7730,7 +7725,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -7743,7 +7738,7 @@
         <v>56</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -7756,7 +7751,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -7769,7 +7764,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -7782,397 +7777,397 @@
         <v>58</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C14" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C15" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C16" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C17" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="C18" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C19" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="C20" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C21" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="C22" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="C23" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="C24" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C25" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="C26" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="C27" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="C28" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="C29" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C30" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C31" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="C32" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="C33" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="27" t="s">
         <v>203</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>204</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="27" t="s">
         <v>206</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>207</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="27" t="s">
         <v>209</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>210</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="27" t="s">
         <v>212</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>213</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="27" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>216</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="27" t="s">
         <v>218</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>219</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="27" t="s">
         <v>221</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>222</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="27" t="s">
         <v>224</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>225</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="27" t="s">
         <v>227</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>228</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="27" t="s">
         <v>230</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>231</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>

</xml_diff>

<commit_message>
next sprint backlog updated
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD77502-8252-45C1-89BD-FDF65D1E9138}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10739D6E-3B90-4360-ACB1-692835DE9789}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20511" yWindow="6051" windowWidth="24686" windowHeight="13149" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8229" yWindow="4766" windowWidth="24685" windowHeight="13148" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="295">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1198,7 +1198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1331,6 +1331,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2113,7 +2114,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2383,7 +2384,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2606,7 +2607,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2829,7 +2830,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3099,7 +3100,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3322,7 +3323,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -4727,8 +4728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="13" customHeight="1"/>
@@ -5457,10 +5458,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
@@ -6038,6 +6039,40 @@
         <v>11</v>
       </c>
       <c r="E36" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A37" s="64">
+        <v>4</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A38" s="64">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
         <v>61</v>
       </c>
     </row>
@@ -8297,7 +8332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Sprint 4 US39 - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/Java/Final Pro/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E6C5FF-E24C-42E0-A875-F4E641A29EB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8229" yWindow="4766" windowWidth="24685" windowHeight="13148" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -24,8 +23,14 @@
     <sheet name="Sprint4" sheetId="9" r:id="rId9"/>
     <sheet name="Stories" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -1065,13 +1070,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
     <numFmt numFmtId="166" formatCode="m&quot;-&quot;yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1462,7 +1467,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1543,7 +1548,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1556,9 +1561,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5539700000000005E-2"/>
-          <c:y val="5.6789800000000001E-2"/>
-          <c:w val="0.89946000000000004"/>
+          <c:x val="0.0955397"/>
+          <c:y val="0.0567898"/>
+          <c:w val="0.89946"/>
           <c:h val="0.838785"/>
         </c:manualLayout>
       </c:layout>
@@ -1602,19 +1607,19 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42060</c:v>
+                  <c:v>42060.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42087</c:v>
+                  <c:v>42087.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42101</c:v>
+                  <c:v>42101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,25 +1631,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AE24-40A1-934F-A0ECF4EAEF47}"/>
             </c:ext>
@@ -1660,17 +1665,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:axId val="-515180352"/>
+        <c:axId val="-515178304"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="-515180352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1698,14 +1703,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="-515178304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="-515178304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="-515180352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -1793,7 +1798,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1806,10 +1811,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.4087399999999998E-2"/>
-          <c:y val="5.6789899999999997E-2"/>
-          <c:w val="0.92091299999999998"/>
-          <c:h val="0.83878399999999997"/>
+          <c:x val="0.0740874"/>
+          <c:y val="0.0567899"/>
+          <c:w val="0.920913"/>
+          <c:h val="0.838784"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1855,16 +1860,16 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42046</c:v>
+                  <c:v>42046.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42059</c:v>
+                  <c:v>42059.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="m/d/yyyy">
-                  <c:v>42087</c:v>
+                <c:pt idx="2" formatCode="m/d/yy">
+                  <c:v>42087.0</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="m/d/yyyy">
-                  <c:v>42101</c:v>
+                <c:pt idx="3" formatCode="m/d/yy">
+                  <c:v>42101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,22 +1881,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-32DE-407F-9CE3-ACCFD4F34A8F}"/>
             </c:ext>
@@ -1907,11 +1912,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094734552"/>
-        <c:axId val="2094734553"/>
+        <c:axId val="-515172688"/>
+        <c:axId val="-515170640"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2094734552"/>
+        <c:axId val="-515172688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,14 +1950,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734553"/>
+        <c:crossAx val="-515170640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2094734553"/>
+        <c:axId val="-515170640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,11 +2002,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094734552"/>
+        <c:crossAx val="-515172688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="5"/>
+        <c:majorUnit val="10.0"/>
+        <c:minorUnit val="5.0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2059,7 +2064,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2095,7 +2100,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2114,7 +2119,7 @@
           <xdr:cNvPr id="3" name="Shape 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2217,7 +2222,7 @@
           <xdr:cNvPr id="4" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2239,7 +2244,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2365,7 +2370,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2384,7 +2389,7 @@
           <xdr:cNvPr id="6" name="Shape 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2487,7 +2492,7 @@
           <xdr:cNvPr id="7" name="Shape 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2509,7 +2514,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2588,7 +2593,7 @@
         <xdr:cNvPr id="11" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2612,7 @@
           <xdr:cNvPr id="9" name="Shape 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2710,7 +2715,7 @@
           <xdr:cNvPr id="10" name="Shape 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2732,7 +2737,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2811,7 +2816,7 @@
         <xdr:cNvPr id="14" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2830,7 +2835,7 @@
           <xdr:cNvPr id="12" name="Shape 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2933,7 +2938,7 @@
           <xdr:cNvPr id="13" name="Shape 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2955,7 +2960,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3081,7 +3086,7 @@
         <xdr:cNvPr id="17" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3100,7 +3105,7 @@
           <xdr:cNvPr id="15" name="Shape 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3203,7 +3208,7 @@
           <xdr:cNvPr id="16" name="Shape 16">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000010000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3225,7 +3230,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3304,7 +3309,7 @@
         <xdr:cNvPr id="20" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3323,7 +3328,7 @@
           <xdr:cNvPr id="18" name="Shape 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000012000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3426,7 +3431,7 @@
           <xdr:cNvPr id="19" name="Shape 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000013000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3448,7 +3453,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3532,7 +3537,7 @@
         <xdr:cNvPr id="22" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4657,33 +4662,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="256" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="50.25" customHeight="1">
+    <row r="3" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="64" t="s">
         <v>0</v>
@@ -4692,28 +4697,28 @@
       <c r="D3" s="65"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -4726,14 +4731,14 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
         <v>4</v>
@@ -4742,7 +4747,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
@@ -4753,7 +4758,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -4762,7 +4767,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -4773,7 +4778,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
         <v>9</v>
@@ -4782,7 +4787,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -4793,7 +4798,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -4802,7 +4807,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
@@ -4813,7 +4818,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -4822,7 +4827,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
@@ -4833,7 +4838,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
@@ -4842,7 +4847,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
@@ -4853,7 +4858,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1">
+    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="8" t="s">
         <v>17</v>
@@ -4862,7 +4867,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="16" customHeight="1">
+    <row r="22" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11" t="s">
@@ -4873,7 +4878,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="16" customHeight="1">
+    <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="8" t="s">
         <v>19</v>
@@ -4882,7 +4887,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="16" customHeight="1">
+    <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
@@ -4893,7 +4898,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1">
+    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="8" t="s">
         <v>21</v>
@@ -4902,7 +4907,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1">
+    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
@@ -4926,20 +4931,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="28.19921875" customWidth="1"/>
-    <col min="3" max="3" width="49.46484375" customWidth="1"/>
-    <col min="4" max="256" width="10.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5" customWidth="1"/>
+    <col min="4" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>51</v>
       </c>
@@ -4952,7 +4959,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="34" customHeight="1">
+    <row r="2" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>64</v>
       </c>
@@ -4965,7 +4972,7 @@
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -4978,7 +4985,7 @@
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>58</v>
       </c>
@@ -4991,7 +4998,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" ht="34" customHeight="1">
+    <row r="5" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>72</v>
       </c>
@@ -5004,7 +5011,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
@@ -5017,7 +5024,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>75</v>
       </c>
@@ -5030,7 +5037,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1">
+    <row r="8" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>60</v>
       </c>
@@ -5043,7 +5050,7 @@
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="34" customHeight="1">
+    <row r="9" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>70</v>
       </c>
@@ -5056,7 +5063,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="34" customHeight="1">
+    <row r="10" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
@@ -5069,7 +5076,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
@@ -5082,7 +5089,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="34" customHeight="1">
+    <row r="12" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>66</v>
       </c>
@@ -5095,7 +5102,7 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" ht="51" customHeight="1">
+    <row r="13" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>79</v>
       </c>
@@ -5108,7 +5115,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="68.25" customHeight="1">
+    <row r="14" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>278</v>
       </c>
@@ -5121,7 +5128,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="34" customHeight="1">
+    <row r="15" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>81</v>
       </c>
@@ -5134,7 +5141,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1">
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>83</v>
       </c>
@@ -5147,7 +5154,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
     </row>
-    <row r="17" spans="1:5" ht="34" customHeight="1">
+    <row r="17" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
@@ -5160,7 +5167,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1">
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>88</v>
       </c>
@@ -5173,7 +5180,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:5" ht="17.25" customHeight="1">
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>90</v>
       </c>
@@ -5186,7 +5193,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1">
+    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>92</v>
       </c>
@@ -5199,7 +5206,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="34" customHeight="1">
+    <row r="21" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>94</v>
       </c>
@@ -5212,7 +5219,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="34" customHeight="1">
+    <row r="22" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>96</v>
       </c>
@@ -5225,7 +5232,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="34" customHeight="1">
+    <row r="23" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>98</v>
       </c>
@@ -5238,7 +5245,7 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="34" customHeight="1">
+    <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>100</v>
       </c>
@@ -5251,7 +5258,7 @@
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="1:5" ht="51" customHeight="1">
+    <row r="25" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>102</v>
       </c>
@@ -5264,7 +5271,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="34" customHeight="1">
+    <row r="26" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
         <v>104</v>
       </c>
@@ -5277,7 +5284,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="136" customHeight="1">
+    <row r="27" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
         <v>106</v>
       </c>
@@ -5290,7 +5297,7 @@
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="17.25" customHeight="1">
+    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>108</v>
       </c>
@@ -5303,7 +5310,7 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="34" customHeight="1">
+    <row r="29" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>110</v>
       </c>
@@ -5316,7 +5323,7 @@
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>112</v>
       </c>
@@ -5329,7 +5336,7 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5" ht="17.25" customHeight="1">
+    <row r="31" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>114</v>
       </c>
@@ -5342,7 +5349,7 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="34" customHeight="1">
+    <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>116</v>
       </c>
@@ -5355,7 +5362,7 @@
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="1:5" ht="17.25" customHeight="1">
+    <row r="33" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
         <v>118</v>
       </c>
@@ -5368,7 +5375,7 @@
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
     </row>
-    <row r="34" spans="1:5" ht="34" customHeight="1">
+    <row r="34" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
         <v>120</v>
       </c>
@@ -5381,7 +5388,7 @@
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
     </row>
-    <row r="35" spans="1:5" ht="51" customHeight="1">
+    <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="18" t="s">
         <v>127</v>
       </c>
@@ -5394,7 +5401,7 @@
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="1:5" ht="34" customHeight="1">
+    <row r="36" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="18" t="s">
         <v>122</v>
       </c>
@@ -5407,7 +5414,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="1:5" ht="34" customHeight="1">
+    <row r="37" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="18" t="s">
         <v>125</v>
       </c>
@@ -5420,7 +5427,7 @@
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="1:5" ht="34" customHeight="1">
+    <row r="38" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="18" t="s">
         <v>303</v>
       </c>
@@ -5433,7 +5440,7 @@
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" ht="34" customHeight="1">
+    <row r="39" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="18" t="s">
         <v>129</v>
       </c>
@@ -5446,7 +5453,7 @@
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" ht="34" customHeight="1">
+    <row r="40" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="18" t="s">
         <v>131</v>
       </c>
@@ -5459,7 +5466,7 @@
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" ht="34" customHeight="1">
+    <row r="41" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="18" t="s">
         <v>308</v>
       </c>
@@ -5472,7 +5479,7 @@
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="1:5" ht="34" customHeight="1">
+    <row r="42" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="18" t="s">
         <v>311</v>
       </c>
@@ -5485,7 +5492,7 @@
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="1:5" ht="34" customHeight="1">
+    <row r="43" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
         <v>314</v>
       </c>
@@ -5508,21 +5515,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.86328125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" customWidth="1"/>
-    <col min="4" max="5" width="20.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
@@ -5539,14 +5546,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>28</v>
       </c>
@@ -5563,7 +5570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
@@ -5580,7 +5587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>38</v>
       </c>
@@ -5597,7 +5604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>43</v>
       </c>
@@ -5614,21 +5621,21 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -5639,7 +5646,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -5656,16 +5663,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.19921875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
@@ -5673,7 +5680,7 @@
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>50</v>
       </c>
@@ -5690,7 +5697,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -5707,7 +5714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -5724,7 +5731,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="19">
         <v>1</v>
       </c>
@@ -5741,7 +5748,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -5758,7 +5765,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19">
         <v>1</v>
       </c>
@@ -5775,7 +5782,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19">
         <v>1</v>
       </c>
@@ -5792,7 +5799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -5809,7 +5816,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19">
         <v>1</v>
       </c>
@@ -5826,7 +5833,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>2</v>
       </c>
@@ -5843,7 +5850,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>74</v>
       </c>
@@ -5860,7 +5867,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>74</v>
       </c>
@@ -5877,7 +5884,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>2</v>
       </c>
@@ -5894,7 +5901,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>74</v>
       </c>
@@ -5911,7 +5918,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19">
         <v>2</v>
       </c>
@@ -5928,7 +5935,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19">
         <v>4</v>
       </c>
@@ -5945,7 +5952,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="19">
         <v>2</v>
       </c>
@@ -5962,7 +5969,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19">
         <v>2</v>
       </c>
@@ -5979,7 +5986,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="19">
         <v>3</v>
       </c>
@@ -5992,7 +5999,7 @@
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="19">
         <v>3</v>
       </c>
@@ -6005,7 +6012,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="19">
         <v>2</v>
       </c>
@@ -6022,7 +6029,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19">
         <v>2</v>
       </c>
@@ -6039,7 +6046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="19">
         <v>4</v>
       </c>
@@ -6056,7 +6063,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="19">
         <v>3</v>
       </c>
@@ -6073,7 +6080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="19">
         <v>4</v>
       </c>
@@ -6090,7 +6097,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="19">
         <v>4</v>
       </c>
@@ -6103,7 +6110,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="19">
         <v>3</v>
       </c>
@@ -6120,7 +6127,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="19">
         <v>4</v>
       </c>
@@ -6133,7 +6140,7 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="19">
         <v>2</v>
       </c>
@@ -6150,7 +6157,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="19">
         <v>3</v>
       </c>
@@ -6167,7 +6174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="19">
         <v>4</v>
       </c>
@@ -6184,7 +6191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="19">
         <v>4</v>
       </c>
@@ -6197,7 +6204,7 @@
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1">
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="19">
         <v>3</v>
       </c>
@@ -6214,7 +6221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="21" customHeight="1">
+    <row r="34" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="23">
         <v>4</v>
       </c>
@@ -6231,7 +6238,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="23">
         <v>4</v>
       </c>
@@ -6248,7 +6255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1">
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="24">
         <v>4</v>
       </c>
@@ -6265,7 +6272,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="27">
         <v>4</v>
       </c>
@@ -6282,7 +6289,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1">
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="30">
         <v>4</v>
       </c>
@@ -6309,23 +6316,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="9.46484375" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" customWidth="1"/>
-    <col min="7" max="256" width="10.86328125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" customHeight="1">
+    <row r="1" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>133</v>
       </c>
@@ -6337,7 +6344,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" ht="13" customHeight="1">
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>134</v>
       </c>
@@ -6349,7 +6356,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
-    <row r="3" spans="1:8" ht="13" customHeight="1">
+    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>135</v>
       </c>
@@ -6361,7 +6368,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:8" ht="13" customHeight="1">
+    <row r="4" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -6371,7 +6378,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:8" ht="13" customHeight="1">
+    <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>136</v>
       </c>
@@ -6383,7 +6390,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="13" customHeight="1">
+    <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>137</v>
       </c>
@@ -6395,7 +6402,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" ht="13" customHeight="1">
+    <row r="7" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6405,7 +6412,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:8" ht="13" customHeight="1">
+    <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>138</v>
       </c>
@@ -6417,7 +6424,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
     </row>
-    <row r="9" spans="1:8" ht="13" customHeight="1">
+    <row r="9" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -6427,7 +6434,7 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="1:8" ht="13" customHeight="1">
+    <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6437,7 +6444,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:8" ht="13" customHeight="1">
+    <row r="11" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6447,7 +6454,7 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" spans="1:8" ht="13" customHeight="1">
+    <row r="12" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -6457,7 +6464,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" ht="13" customHeight="1">
+    <row r="13" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -6467,7 +6474,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" ht="13" customHeight="1">
+    <row r="14" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
@@ -6491,7 +6498,7 @@
       </c>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1">
+    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>145</v>
       </c>
@@ -6509,7 +6516,7 @@
       <c r="G15" s="37"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="13" customHeight="1">
+    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>146</v>
       </c>
@@ -6535,7 +6542,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="13" customHeight="1">
+    <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>147</v>
       </c>
@@ -6561,7 +6568,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="13" customHeight="1">
+    <row r="18" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>148</v>
       </c>
@@ -6587,7 +6594,7 @@
       </c>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="13" customHeight="1">
+    <row r="19" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>149</v>
       </c>
@@ -6611,7 +6618,7 @@
       </c>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="13" customHeight="1">
+    <row r="20" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="30"/>
@@ -6621,7 +6628,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="13" customHeight="1">
+    <row r="21" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -6631,7 +6638,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="13" customHeight="1">
+    <row r="22" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -6641,7 +6648,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="13" customHeight="1">
+    <row r="23" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -6651,7 +6658,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" ht="13" customHeight="1">
+    <row r="24" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -6661,7 +6668,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" ht="13" customHeight="1">
+    <row r="25" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -6671,7 +6678,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="13" customHeight="1">
+    <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -6681,7 +6688,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="13" customHeight="1">
+    <row r="27" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -6691,7 +6698,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="1:8" ht="13" customHeight="1">
+    <row r="28" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -6701,7 +6708,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="1:8" ht="13" customHeight="1">
+    <row r="29" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -6711,7 +6718,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="13" customHeight="1">
+    <row r="30" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -6721,7 +6728,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="13" customHeight="1">
+    <row r="31" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -6731,7 +6738,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1">
+    <row r="32" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -6741,7 +6748,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="13" customHeight="1">
+    <row r="33" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -6751,7 +6758,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
     </row>
-    <row r="34" spans="1:8" ht="13" customHeight="1">
+    <row r="34" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -6761,7 +6768,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:8" ht="13" customHeight="1">
+    <row r="35" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -6771,7 +6778,7 @@
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8" ht="13" customHeight="1">
+    <row r="36" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
@@ -6781,7 +6788,7 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
     </row>
-    <row r="37" spans="1:8" ht="13" customHeight="1">
+    <row r="37" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -6791,7 +6798,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8" ht="13" customHeight="1">
+    <row r="38" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="19"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -6801,7 +6808,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="13" customHeight="1">
+    <row r="39" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -6822,23 +6829,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="4" width="7.19921875" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" customWidth="1"/>
-    <col min="7" max="256" width="10.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1">
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>139</v>
       </c>
@@ -6859,7 +6866,7 @@
       </c>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1">
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="39">
         <v>42046</v>
       </c>
@@ -6874,7 +6881,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="13" customHeight="1">
+    <row r="3" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="39">
         <v>42059</v>
       </c>
@@ -6897,7 +6904,7 @@
       </c>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="13" customHeight="1">
+    <row r="4" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="41">
         <v>42087</v>
       </c>
@@ -6918,7 +6925,7 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="13" customHeight="1">
+    <row r="5" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="41">
         <v>42101</v>
       </c>
@@ -6939,7 +6946,7 @@
       </c>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="13" customHeight="1">
+    <row r="6" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -6948,7 +6955,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="13" customHeight="1">
+    <row r="7" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6957,7 +6964,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="13" customHeight="1">
+    <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -6966,7 +6973,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="13" customHeight="1">
+    <row r="9" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -6975,7 +6982,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" ht="13" customHeight="1">
+    <row r="10" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6984,7 +6991,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" ht="13" customHeight="1">
+    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6993,7 +7000,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" ht="13" customHeight="1">
+    <row r="12" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -7002,7 +7009,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:7" ht="13" customHeight="1">
+    <row r="13" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -7011,7 +7018,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:7" ht="13" customHeight="1">
+    <row r="14" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -7020,7 +7027,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" ht="13" customHeight="1">
+    <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -7029,7 +7036,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:7" ht="13" customHeight="1">
+    <row r="16" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -7038,7 +7045,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="1:7" ht="13" customHeight="1">
+    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -7047,7 +7054,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" ht="13" customHeight="1">
+    <row r="18" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -7056,7 +7063,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" ht="13" customHeight="1">
+    <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -7065,7 +7072,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="13" customHeight="1">
+    <row r="20" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -7074,7 +7081,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="13" customHeight="1">
+    <row r="21" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -7083,7 +7090,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="13" customHeight="1">
+    <row r="22" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -7092,7 +7099,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
     </row>
-    <row r="23" spans="1:7" ht="13" customHeight="1">
+    <row r="23" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -7101,7 +7108,7 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="13" customHeight="1">
+    <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -7110,7 +7117,7 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="13" customHeight="1">
+    <row r="25" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -7119,7 +7126,7 @@
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="13" customHeight="1">
+    <row r="26" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -7139,33 +7146,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="8.46484375" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.46484375" customWidth="1"/>
-    <col min="12" max="12" width="19.19921875" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.86328125" customWidth="1"/>
-    <col min="15" max="15" width="10.19921875" customWidth="1"/>
-    <col min="16" max="16" width="16.46484375" customWidth="1"/>
-    <col min="17" max="17" width="10.19921875" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
@@ -7214,7 +7221,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1">
+    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>55</v>
       </c>
@@ -7263,7 +7270,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1">
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>58</v>
       </c>
@@ -7312,7 +7319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" customHeight="1">
+    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>60</v>
       </c>
@@ -7361,7 +7368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" customHeight="1">
+    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>62</v>
       </c>
@@ -7410,7 +7417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1">
+    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>64</v>
       </c>
@@ -7459,7 +7466,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1">
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>66</v>
       </c>
@@ -7508,7 +7515,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1">
+    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>68</v>
       </c>
@@ -7557,7 +7564,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17.25" customHeight="1">
+    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>70</v>
       </c>
@@ -7606,7 +7613,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10" s="47"/>
       <c r="C10" s="19"/>
@@ -7625,7 +7632,7 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19"/>
       <c r="B11" s="47"/>
       <c r="C11" s="19"/>
@@ -7644,7 +7651,7 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19"/>
       <c r="B12" s="47"/>
       <c r="C12" s="19"/>
@@ -7663,7 +7670,7 @@
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19"/>
       <c r="B13" s="47"/>
       <c r="C13" s="19"/>
@@ -7682,7 +7689,7 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="19"/>
       <c r="B14" s="42" t="s">
         <v>192</v>
@@ -7703,7 +7710,7 @@
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19"/>
       <c r="B15" s="42"/>
       <c r="C15" s="19"/>
@@ -7722,7 +7729,7 @@
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19"/>
       <c r="B16" s="42" t="s">
         <v>193</v>
@@ -7745,7 +7752,7 @@
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1">
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="19"/>
       <c r="B17" s="47"/>
       <c r="C17" s="18" t="s">
@@ -7766,7 +7773,7 @@
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1">
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19"/>
       <c r="B18" s="47"/>
       <c r="C18" s="18" t="s">
@@ -7787,7 +7794,7 @@
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="19"/>
       <c r="B19" s="47"/>
       <c r="C19" s="19"/>
@@ -7806,7 +7813,7 @@
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1">
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="19"/>
       <c r="B20" s="42" t="s">
         <v>197</v>
@@ -7839,12 +7846,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
@@ -7857,7 +7864,7 @@
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5" customHeight="1">
+    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
@@ -7906,7 +7913,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>96</v>
       </c>
@@ -7955,7 +7962,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>98</v>
       </c>
@@ -8004,7 +8011,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>83</v>
       </c>
@@ -8053,7 +8060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>72</v>
       </c>
@@ -8102,7 +8109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>90</v>
       </c>
@@ -8151,7 +8158,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>112</v>
       </c>
@@ -8200,7 +8207,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>88</v>
       </c>
@@ -8249,7 +8256,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1">
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>79</v>
       </c>
@@ -8298,7 +8305,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -8317,7 +8324,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -8336,7 +8343,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
@@ -8355,7 +8362,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="14.25" customHeight="1">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="27"/>
       <c r="B13" s="42" t="s">
         <v>192</v>
@@ -8376,7 +8383,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="14.25" customHeight="1">
+    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="27"/>
       <c r="B14" s="42"/>
       <c r="C14" s="19"/>
@@ -8395,7 +8402,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1">
+    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="27"/>
       <c r="B15" s="42" t="s">
         <v>193</v>
@@ -8418,7 +8425,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" customHeight="1">
+    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="27"/>
       <c r="B16" s="47"/>
       <c r="C16" s="18" t="s">
@@ -8439,7 +8446,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="1:17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
       <c r="B17" s="47"/>
       <c r="C17" s="18"/>
@@ -8458,7 +8465,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="1:17" ht="14.25" customHeight="1">
+    <row r="18" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="27"/>
       <c r="B18" s="47"/>
       <c r="C18" s="19"/>
@@ -8477,7 +8484,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" ht="14.25" customHeight="1">
+    <row r="19" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="27"/>
       <c r="B19" s="42" t="s">
         <v>197</v>
@@ -8500,7 +8507,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" ht="14.25" customHeight="1">
+    <row r="20" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="33" t="s">
@@ -8521,7 +8528,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="14.25" customHeight="1">
+    <row r="21" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13"/>
       <c r="B21" s="17"/>
       <c r="C21" s="49" t="s">
@@ -8552,22 +8559,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="20.46484375" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.5" customHeight="1">
+    <row r="1" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="50" t="s">
         <v>51</v>
       </c>
@@ -8615,7 +8622,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
         <v>77</v>
       </c>
@@ -8663,7 +8670,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="54" t="s">
         <v>102</v>
       </c>
@@ -8711,7 +8718,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="54" t="s">
         <v>81</v>
       </c>
@@ -8759,7 +8766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="54" t="s">
         <v>75</v>
       </c>
@@ -8807,7 +8814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="54" t="s">
         <v>116</v>
       </c>
@@ -8855,7 +8862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="54" t="s">
         <v>120</v>
       </c>
@@ -8903,7 +8910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="54" t="s">
         <v>108</v>
       </c>
@@ -8951,7 +8958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="54" t="s">
         <v>114</v>
       </c>
@@ -8999,7 +9006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="53"/>
       <c r="B10" s="53"/>
       <c r="C10" s="53"/>
@@ -9017,7 +9024,7 @@
       <c r="O10" s="59"/>
       <c r="P10" s="60"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -9035,7 +9042,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -9053,7 +9060,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -9071,7 +9078,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
@@ -9089,7 +9096,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:16" ht="14.25" customHeight="1">
+    <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="27"/>
       <c r="B15" s="42" t="s">
         <v>192</v>
@@ -9109,7 +9116,7 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="27"/>
       <c r="B16" s="42"/>
       <c r="C16" s="19"/>
@@ -9127,7 +9134,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="1:16" ht="14.25" customHeight="1">
+    <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
       <c r="B17" s="42" t="s">
         <v>193</v>
@@ -9149,7 +9156,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" ht="14.25" customHeight="1">
+    <row r="18" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="27"/>
       <c r="B18" s="47"/>
       <c r="C18" s="18" t="s">
@@ -9169,7 +9176,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:16" ht="14.25" customHeight="1">
+    <row r="19" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="27"/>
       <c r="B19" s="47"/>
       <c r="C19" s="18"/>
@@ -9187,7 +9194,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:16" ht="14.25" customHeight="1">
+    <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="27"/>
       <c r="B20" s="47"/>
       <c r="C20" s="19"/>
@@ -9205,7 +9212,7 @@
       <c r="O20" s="5"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:16" ht="14.25" customHeight="1">
+    <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="27"/>
       <c r="B21" s="42" t="s">
         <v>197</v>
@@ -9227,7 +9234,7 @@
       <c r="O21" s="5"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:16" ht="14.25" customHeight="1">
+    <row r="22" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="33" t="s">
@@ -9247,7 +9254,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="1:16" ht="14.25" customHeight="1">
+    <row r="23" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13"/>
       <c r="B23" s="17"/>
       <c r="C23" s="49" t="s">
@@ -9277,19 +9284,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="10.86328125" customWidth="1"/>
+    <col min="1" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" customHeight="1">
+    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="42" t="s">
         <v>51</v>
       </c>
@@ -9318,7 +9325,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="26.25" customHeight="1">
+    <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="62" t="s">
         <v>122</v>
       </c>
@@ -9341,7 +9348,7 @@
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
     </row>
-    <row r="3" spans="1:9" ht="26.25" customHeight="1">
+    <row r="3" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="62" t="s">
         <v>125</v>
       </c>
@@ -9364,7 +9371,7 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="62" t="s">
         <v>104</v>
       </c>
@@ -9387,7 +9394,7 @@
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="62" t="s">
         <v>131</v>
       </c>
@@ -9410,7 +9417,7 @@
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="62" t="s">
         <v>85</v>
       </c>
@@ -9433,7 +9440,7 @@
       <c r="H6" s="47"/>
       <c r="I6" s="47"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="62" t="s">
         <v>100</v>
       </c>
@@ -9456,7 +9463,7 @@
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>127</v>
       </c>
@@ -9479,7 +9486,7 @@
       <c r="H8" s="47"/>
       <c r="I8" s="47"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>129</v>
       </c>
@@ -9502,7 +9509,7 @@
       <c r="H9" s="47"/>
       <c r="I9" s="47"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>

</xml_diff>

<commit_message>
Added Sprint 4 US39 and its test cases - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -4934,8 +4934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5666,8 +5666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:E37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6303,7 +6303,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected Gedcom Test input file - test data was overwritten. Updated Team xlsx sheet for US35 and US36
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens\Courses\CS-555-Agile Methods for SW Eng\GEDCOMProject\CS_555_JAVS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A7AD15-F988-4AFA-91DF-DDE164E979EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0290669-7099-4AB2-B4D6-AF4AF484DBCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="333">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1087,6 +1087,35 @@
   </si>
   <si>
     <t>test_US38listOfUpcomingBirthdays</t>
+  </si>
+  <si>
+    <t>US35_findListOfRecentBirths</t>
+  </si>
+  <si>
+    <t>US36_findListOfRecentDeaths</t>
+  </si>
+  <si>
+    <t>124-140</t>
+  </si>
+  <si>
+    <t>test_US35ListOfRecentBirthsSuccess,
+test_US35ListOfRecentBirthsFailure</t>
+  </si>
+  <si>
+    <t>283-345</t>
+  </si>
+  <si>
+    <t>143-159</t>
+  </si>
+  <si>
+    <t>test_US36ListOfRecentDeathsSuccess,
+test_US35ListOfRecentDeathsFailure</t>
+  </si>
+  <si>
+    <t>347-409</t>
+  </si>
+  <si>
+    <t>Avoid inegration at the end, Avoid editing other US's test data in gedcom file-create your own test data</t>
   </si>
 </sst>
 </file>
@@ -2131,8 +2160,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1287162" y="1289863"/>
-          <a:ext cx="1504144" cy="1066774"/>
+          <a:off x="1220487" y="1267638"/>
+          <a:ext cx="1446994" cy="1044549"/>
           <a:chOff x="-19049" y="-41148"/>
           <a:chExt cx="1446994" cy="1066774"/>
         </a:xfrm>
@@ -2267,7 +2296,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2401,8 +2430,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5631597" y="1308961"/>
-          <a:ext cx="1433836" cy="792204"/>
+          <a:off x="5209322" y="1286736"/>
+          <a:ext cx="1367161" cy="776329"/>
           <a:chOff x="-19051" y="-41148"/>
           <a:chExt cx="1363986" cy="792204"/>
         </a:xfrm>
@@ -2537,7 +2566,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2624,8 +2653,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2839718" y="1090477"/>
-          <a:ext cx="1355515" cy="1077925"/>
+          <a:off x="2715893" y="1071427"/>
+          <a:ext cx="1174540" cy="1055700"/>
           <a:chOff x="-19050" y="-52578"/>
           <a:chExt cx="1177716" cy="1077924"/>
         </a:xfrm>
@@ -2760,7 +2789,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2847,8 +2876,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4048094" y="1451911"/>
-          <a:ext cx="579784" cy="666702"/>
+          <a:off x="3743294" y="1426511"/>
+          <a:ext cx="538509" cy="654002"/>
           <a:chOff x="-19050" y="-31618"/>
           <a:chExt cx="535334" cy="666701"/>
         </a:xfrm>
@@ -2983,7 +3012,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3117,8 +3146,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4465317" y="1111643"/>
-          <a:ext cx="1353399" cy="1133467"/>
+          <a:off x="4160517" y="1092593"/>
+          <a:ext cx="1235924" cy="1111242"/>
           <a:chOff x="-19050" y="-52578"/>
           <a:chExt cx="1232748" cy="1133467"/>
         </a:xfrm>
@@ -3253,7 +3282,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3340,8 +3369,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5784323" y="4949628"/>
-          <a:ext cx="1408429" cy="995923"/>
+          <a:off x="5362048" y="4857553"/>
+          <a:ext cx="1341754" cy="973698"/>
           <a:chOff x="-19051" y="-41148"/>
           <a:chExt cx="1338579" cy="995923"/>
         </a:xfrm>
@@ -3476,7 +3505,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -4688,14 +4717,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.69140625" customWidth="1"/>
+    <col min="2" max="4" width="33.75" customWidth="1"/>
     <col min="5" max="256" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4763,7 +4792,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" spans="1:5" ht="15.95" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
         <v>4</v>
@@ -4772,7 +4801,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" spans="1:5" ht="15.95" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
@@ -4783,7 +4812,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" spans="1:5" ht="15.95" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -4792,7 +4821,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" spans="1:5" ht="15.95" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -4803,7 +4832,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" spans="1:5" ht="15.95" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
         <v>9</v>
@@ -4812,7 +4841,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" spans="1:5" ht="15.95" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -4823,7 +4852,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+    <row r="15" spans="1:5" ht="15.95" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -4832,7 +4861,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" spans="1:5" ht="15.95" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
@@ -4843,7 +4872,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1">
+    <row r="17" spans="1:5" ht="15.95" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -4852,7 +4881,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1">
+    <row r="18" spans="1:5" ht="15.95" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
@@ -4863,7 +4892,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1">
+    <row r="19" spans="1:5" ht="15.95" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
@@ -4872,7 +4901,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1">
+    <row r="20" spans="1:5" ht="15.95" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
@@ -4883,7 +4912,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1">
+    <row r="21" spans="1:5" ht="15.95" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="8" t="s">
         <v>17</v>
@@ -4892,7 +4921,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="16" customHeight="1">
+    <row r="22" spans="1:5" ht="15.95" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11" t="s">
@@ -4903,7 +4932,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="16" customHeight="1">
+    <row r="23" spans="1:5" ht="15.95" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" s="8" t="s">
         <v>19</v>
@@ -4912,7 +4941,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="16" customHeight="1">
+    <row r="24" spans="1:5" ht="15.95" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
@@ -4923,7 +4952,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1">
+    <row r="25" spans="1:5" ht="15.95" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="8" t="s">
         <v>21</v>
@@ -4932,7 +4961,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1">
+    <row r="26" spans="1:5" ht="15.95" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
@@ -4963,12 +4992,12 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.84375" customWidth="1"/>
-    <col min="2" max="2" width="28.15234375" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" customWidth="1"/>
-    <col min="4" max="256" width="10.84375" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="3" max="3" width="49.5" customWidth="1"/>
+    <col min="4" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
@@ -4984,7 +5013,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="34" customHeight="1">
+    <row r="2" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>64</v>
       </c>
@@ -5023,7 +5052,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" ht="34" customHeight="1">
+    <row r="5" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>72</v>
       </c>
@@ -5075,7 +5104,7 @@
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="34" customHeight="1">
+    <row r="9" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>70</v>
       </c>
@@ -5088,7 +5117,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="34" customHeight="1">
+    <row r="10" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
@@ -5101,7 +5130,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
@@ -5114,7 +5143,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="34" customHeight="1">
+    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>66</v>
       </c>
@@ -5153,7 +5182,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="34" customHeight="1">
+    <row r="15" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>81</v>
       </c>
@@ -5179,7 +5208,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
     </row>
-    <row r="17" spans="1:5" ht="34" customHeight="1">
+    <row r="17" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
@@ -5231,7 +5260,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="34" customHeight="1">
+    <row r="21" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>94</v>
       </c>
@@ -5244,7 +5273,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="34" customHeight="1">
+    <row r="22" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>96</v>
       </c>
@@ -5257,7 +5286,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="34" customHeight="1">
+    <row r="23" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A23" s="18" t="s">
         <v>98</v>
       </c>
@@ -5270,7 +5299,7 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="34" customHeight="1">
+    <row r="24" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>100</v>
       </c>
@@ -5296,7 +5325,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="34" customHeight="1">
+    <row r="26" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A26" s="18" t="s">
         <v>104</v>
       </c>
@@ -5309,7 +5338,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="136" customHeight="1">
+    <row r="27" spans="1:5" ht="135.94999999999999" customHeight="1">
       <c r="A27" s="18" t="s">
         <v>106</v>
       </c>
@@ -5335,7 +5364,7 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="34" customHeight="1">
+    <row r="29" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A29" s="18" t="s">
         <v>110</v>
       </c>
@@ -5374,7 +5403,7 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="34" customHeight="1">
+    <row r="32" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A32" s="18" t="s">
         <v>116</v>
       </c>
@@ -5400,7 +5429,7 @@
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
     </row>
-    <row r="34" spans="1:5" ht="34" customHeight="1">
+    <row r="34" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A34" s="18" t="s">
         <v>120</v>
       </c>
@@ -5426,7 +5455,7 @@
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="1:5" ht="34" customHeight="1">
+    <row r="36" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A36" s="18" t="s">
         <v>122</v>
       </c>
@@ -5439,7 +5468,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="1:5" ht="34" customHeight="1">
+    <row r="37" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A37" s="18" t="s">
         <v>125</v>
       </c>
@@ -5452,7 +5481,7 @@
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="1:5" ht="34" customHeight="1">
+    <row r="38" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A38" s="18" t="s">
         <v>303</v>
       </c>
@@ -5465,7 +5494,7 @@
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" ht="34" customHeight="1">
+    <row r="39" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A39" s="18" t="s">
         <v>129</v>
       </c>
@@ -5478,7 +5507,7 @@
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" ht="34" customHeight="1">
+    <row r="40" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A40" s="18" t="s">
         <v>131</v>
       </c>
@@ -5491,7 +5520,7 @@
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" ht="34" customHeight="1">
+    <row r="41" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A41" s="18" t="s">
         <v>308</v>
       </c>
@@ -5504,7 +5533,7 @@
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="1:5" ht="34" customHeight="1">
+    <row r="42" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A42" s="18" t="s">
         <v>311</v>
       </c>
@@ -5517,7 +5546,7 @@
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="1:5" ht="34" customHeight="1">
+    <row r="43" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A43" s="18" t="s">
         <v>314</v>
       </c>
@@ -5547,10 +5576,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.84375" customWidth="1"/>
-    <col min="2" max="2" width="10.69140625" customWidth="1"/>
-    <col min="3" max="3" width="10.84375" customWidth="1"/>
-    <col min="4" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5691,17 +5720,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.15234375" customWidth="1"/>
-    <col min="2" max="2" width="7.69140625" customWidth="1"/>
-    <col min="3" max="3" width="25.3046875" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" customWidth="1"/>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="3" max="3" width="25.25" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6260,7 +6289,7 @@
         <v>124</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -6277,7 +6306,7 @@
         <v>28</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
@@ -6346,18 +6375,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.84375" customWidth="1"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" customWidth="1"/>
-    <col min="7" max="256" width="10.84375" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" customHeight="1">
+    <row r="1" spans="1:8" ht="12.95" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>133</v>
       </c>
@@ -6369,7 +6398,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" ht="13" customHeight="1">
+    <row r="2" spans="1:8" ht="12.95" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>134</v>
       </c>
@@ -6381,7 +6410,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
-    <row r="3" spans="1:8" ht="13" customHeight="1">
+    <row r="3" spans="1:8" ht="12.95" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>135</v>
       </c>
@@ -6393,7 +6422,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:8" ht="13" customHeight="1">
+    <row r="4" spans="1:8" ht="12.95" customHeight="1">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -6403,7 +6432,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:8" ht="13" customHeight="1">
+    <row r="5" spans="1:8" ht="12.95" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>136</v>
       </c>
@@ -6415,7 +6444,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="13" customHeight="1">
+    <row r="6" spans="1:8" ht="12.95" customHeight="1">
       <c r="A6" s="18" t="s">
         <v>137</v>
       </c>
@@ -6427,7 +6456,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" ht="13" customHeight="1">
+    <row r="7" spans="1:8" ht="12.95" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6437,7 +6466,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:8" ht="13" customHeight="1">
+    <row r="8" spans="1:8" ht="12.95" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>138</v>
       </c>
@@ -6449,7 +6478,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
     </row>
-    <row r="9" spans="1:8" ht="13" customHeight="1">
+    <row r="9" spans="1:8" ht="12.95" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -6459,7 +6488,7 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="1:8" ht="13" customHeight="1">
+    <row r="10" spans="1:8" ht="12.95" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6469,7 +6498,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:8" ht="13" customHeight="1">
+    <row r="11" spans="1:8" ht="12.95" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6479,7 +6508,7 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" spans="1:8" ht="13" customHeight="1">
+    <row r="12" spans="1:8" ht="12.95" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -6489,7 +6518,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" ht="13" customHeight="1">
+    <row r="13" spans="1:8" ht="12.95" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -6499,7 +6528,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" ht="13" customHeight="1">
+    <row r="14" spans="1:8" ht="12.95" customHeight="1">
       <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
@@ -6523,7 +6552,7 @@
       </c>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1">
+    <row r="15" spans="1:8" ht="12.95" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>145</v>
       </c>
@@ -6541,7 +6570,7 @@
       <c r="G15" s="37"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="13" customHeight="1">
+    <row r="16" spans="1:8" ht="12.95" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>146</v>
       </c>
@@ -6567,7 +6596,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="13" customHeight="1">
+    <row r="17" spans="1:8" ht="12.95" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>147</v>
       </c>
@@ -6593,7 +6622,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="13" customHeight="1">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>148</v>
       </c>
@@ -6619,7 +6648,7 @@
       </c>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="13" customHeight="1">
+    <row r="19" spans="1:8" ht="12.95" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>149</v>
       </c>
@@ -6643,7 +6672,7 @@
       </c>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="13" customHeight="1">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="30"/>
@@ -6653,7 +6682,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="13" customHeight="1">
+    <row r="21" spans="1:8" ht="12.95" customHeight="1">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -6663,7 +6692,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="13" customHeight="1">
+    <row r="22" spans="1:8" ht="12.95" customHeight="1">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -6673,7 +6702,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="13" customHeight="1">
+    <row r="23" spans="1:8" ht="12.95" customHeight="1">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -6683,7 +6712,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" ht="13" customHeight="1">
+    <row r="24" spans="1:8" ht="12.95" customHeight="1">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -6693,7 +6722,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" ht="13" customHeight="1">
+    <row r="25" spans="1:8" ht="12.95" customHeight="1">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -6703,7 +6732,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="13" customHeight="1">
+    <row r="26" spans="1:8" ht="12.95" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -6713,7 +6742,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="13" customHeight="1">
+    <row r="27" spans="1:8" ht="12.95" customHeight="1">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -6723,7 +6752,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="1:8" ht="13" customHeight="1">
+    <row r="28" spans="1:8" ht="12.95" customHeight="1">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -6733,7 +6762,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="1:8" ht="13" customHeight="1">
+    <row r="29" spans="1:8" ht="12.95" customHeight="1">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -6743,7 +6772,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="13" customHeight="1">
+    <row r="30" spans="1:8" ht="12.95" customHeight="1">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -6753,7 +6782,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="13" customHeight="1">
+    <row r="31" spans="1:8" ht="12.95" customHeight="1">
       <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -6763,7 +6792,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1">
+    <row r="32" spans="1:8" ht="12.95" customHeight="1">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -6773,7 +6802,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="13" customHeight="1">
+    <row r="33" spans="1:8" ht="12.95" customHeight="1">
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -6783,7 +6812,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
     </row>
-    <row r="34" spans="1:8" ht="13" customHeight="1">
+    <row r="34" spans="1:8" ht="12.95" customHeight="1">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -6793,7 +6822,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:8" ht="13" customHeight="1">
+    <row r="35" spans="1:8" ht="12.95" customHeight="1">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -6803,7 +6832,7 @@
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8" ht="13" customHeight="1">
+    <row r="36" spans="1:8" ht="12.95" customHeight="1">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
@@ -6813,7 +6842,7 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
     </row>
-    <row r="37" spans="1:8" ht="13" customHeight="1">
+    <row r="37" spans="1:8" ht="12.95" customHeight="1">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -6823,7 +6852,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8" ht="13" customHeight="1">
+    <row r="38" spans="1:8" ht="12.95" customHeight="1">
       <c r="A38" s="19"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -6833,7 +6862,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="13" customHeight="1">
+    <row r="39" spans="1:8" ht="12.95" customHeight="1">
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -6857,20 +6886,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.84375" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" customWidth="1"/>
-    <col min="7" max="256" width="10.84375" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1">
+    <row r="1" spans="1:7" ht="12.95" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>139</v>
       </c>
@@ -6891,7 +6922,7 @@
       </c>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1">
+    <row r="2" spans="1:7" ht="12.95" customHeight="1">
       <c r="A2" s="39">
         <v>42046</v>
       </c>
@@ -6906,7 +6937,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="13" customHeight="1">
+    <row r="3" spans="1:7" ht="12.95" customHeight="1">
       <c r="A3" s="39">
         <v>42059</v>
       </c>
@@ -6929,7 +6960,7 @@
       </c>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="13" customHeight="1">
+    <row r="4" spans="1:7" ht="12.95" customHeight="1">
       <c r="A4" s="41">
         <v>42087</v>
       </c>
@@ -6950,7 +6981,7 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="13" customHeight="1">
+    <row r="5" spans="1:7" ht="12.95" customHeight="1">
       <c r="A5" s="41">
         <v>42101</v>
       </c>
@@ -6971,7 +7002,7 @@
       </c>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="13" customHeight="1">
+    <row r="6" spans="1:7" ht="12.95" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -6980,7 +7011,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="13" customHeight="1">
+    <row r="7" spans="1:7" ht="12.95" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6989,7 +7020,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="13" customHeight="1">
+    <row r="8" spans="1:7" ht="12.95" customHeight="1">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -6998,7 +7029,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="13" customHeight="1">
+    <row r="9" spans="1:7" ht="12.95" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -7007,7 +7038,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" ht="13" customHeight="1">
+    <row r="10" spans="1:7" ht="12.95" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -7016,7 +7047,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" ht="13" customHeight="1">
+    <row r="11" spans="1:7" ht="12.95" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -7025,7 +7056,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" ht="13" customHeight="1">
+    <row r="12" spans="1:7" ht="12.95" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -7034,7 +7065,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:7" ht="13" customHeight="1">
+    <row r="13" spans="1:7" ht="12.95" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -7043,7 +7074,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:7" ht="13" customHeight="1">
+    <row r="14" spans="1:7" ht="12.95" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -7052,7 +7083,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" ht="13" customHeight="1">
+    <row r="15" spans="1:7" ht="12.95" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -7061,7 +7092,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:7" ht="13" customHeight="1">
+    <row r="16" spans="1:7" ht="12.95" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -7070,7 +7101,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="1:7" ht="13" customHeight="1">
+    <row r="17" spans="1:7" ht="12.95" customHeight="1">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -7079,7 +7110,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" ht="13" customHeight="1">
+    <row r="18" spans="1:7" ht="12.95" customHeight="1">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -7088,7 +7119,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" ht="13" customHeight="1">
+    <row r="19" spans="1:7" ht="12.95" customHeight="1">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -7097,7 +7128,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="13" customHeight="1">
+    <row r="20" spans="1:7" ht="12.95" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -7106,7 +7137,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="13" customHeight="1">
+    <row r="21" spans="1:7" ht="12.95" customHeight="1">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -7115,7 +7146,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="13" customHeight="1">
+    <row r="22" spans="1:7" ht="12.95" customHeight="1">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -7124,7 +7155,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
     </row>
-    <row r="23" spans="1:7" ht="13" customHeight="1">
+    <row r="23" spans="1:7" ht="12.95" customHeight="1">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -7133,7 +7164,7 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="13" customHeight="1">
+    <row r="24" spans="1:7" ht="12.95" customHeight="1">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -7142,7 +7173,7 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="13" customHeight="1">
+    <row r="25" spans="1:7" ht="12.95" customHeight="1">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -7151,7 +7182,7 @@
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="13" customHeight="1">
+    <row r="26" spans="1:7" ht="12.95" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -7178,22 +7209,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" customWidth="1"/>
-    <col min="3" max="3" width="7.3046875" customWidth="1"/>
-    <col min="4" max="4" width="8.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" customWidth="1"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="9.25" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.4609375" customWidth="1"/>
-    <col min="12" max="12" width="19.15234375" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="19.125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.84375" customWidth="1"/>
-    <col min="15" max="15" width="10.15234375" customWidth="1"/>
-    <col min="16" max="16" width="16.4609375" customWidth="1"/>
-    <col min="17" max="17" width="10.15234375" customWidth="1"/>
+    <col min="14" max="14" width="1.875" customWidth="1"/>
+    <col min="15" max="15" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="10.125" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7879,12 +7910,12 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="20.69140625" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="22.69140625" customWidth="1"/>
+    <col min="12" max="12" width="22.75" customWidth="1"/>
     <col min="13" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="19.3046875" customWidth="1"/>
-    <col min="16" max="16" width="190.69140625" customWidth="1"/>
+    <col min="15" max="15" width="19.25" customWidth="1"/>
+    <col min="16" max="16" width="190.75" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
@@ -8594,9 +8625,9 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="22.69140625" customWidth="1"/>
+    <col min="2" max="2" width="22.75" customWidth="1"/>
     <col min="3" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="20.4609375" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="256" width="11" customWidth="1"/>
   </cols>
@@ -9315,15 +9346,15 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="10.84375" customWidth="1"/>
+    <col min="1" max="256" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28" customHeight="1">
+    <row r="1" spans="1:16" ht="27.95" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>51</v>
       </c>
@@ -9390,16 +9421,34 @@
       <c r="F2" s="47">
         <v>60</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
+      <c r="G2" s="47">
+        <v>16</v>
+      </c>
+      <c r="H2" s="47">
+        <v>30</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>324</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>326</v>
+      </c>
       <c r="M2" s="53"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="55"/>
+      <c r="N2" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="O2" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
       <c r="A3" s="62" t="s">
@@ -9420,16 +9469,34 @@
       <c r="F3" s="47">
         <v>60</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
+      <c r="G3" s="47">
+        <v>16</v>
+      </c>
+      <c r="H3" s="47">
+        <v>30</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>325</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>329</v>
+      </c>
       <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="55"/>
+      <c r="N3" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="O3" s="54" t="s">
+        <v>330</v>
+      </c>
+      <c r="P3" s="55" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="62" t="s">
@@ -9658,7 +9725,7 @@
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
     </row>
-    <row r="17" spans="3:9" ht="13" customHeight="1">
+    <row r="17" spans="3:9" ht="12.95" customHeight="1">
       <c r="C17" s="42" t="s">
         <v>192</v>
       </c>
@@ -9669,7 +9736,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="3:9" ht="13" customHeight="1">
+    <row r="18" spans="3:9" ht="12.95" customHeight="1">
       <c r="C18" s="42"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -9678,7 +9745,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="3:9" ht="13" customHeight="1">
+    <row r="19" spans="3:9" ht="12.95" customHeight="1">
       <c r="C19" s="42" t="s">
         <v>193</v>
       </c>
@@ -9691,7 +9758,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="3:9" ht="13" customHeight="1">
+    <row r="20" spans="3:9" ht="12.95" customHeight="1">
       <c r="C20" s="47"/>
       <c r="D20" s="18" t="s">
         <v>260</v>
@@ -9702,7 +9769,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="3:9" ht="13" customHeight="1">
+    <row r="21" spans="3:9" ht="12.95" customHeight="1">
       <c r="C21" s="47"/>
       <c r="D21" s="18"/>
       <c r="E21" s="19"/>
@@ -9711,7 +9778,7 @@
       <c r="H21" s="19"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="3:9" ht="13" customHeight="1">
+    <row r="22" spans="3:9" ht="12.95" customHeight="1">
       <c r="C22" s="47"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
@@ -9720,7 +9787,7 @@
       <c r="H22" s="19"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="3:9" ht="13" customHeight="1">
+    <row r="23" spans="3:9" ht="12.95" customHeight="1">
       <c r="C23" s="42" t="s">
         <v>197</v>
       </c>
@@ -9733,10 +9800,10 @@
       <c r="H23" s="19"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="3:9" ht="13" customHeight="1">
+    <row r="24" spans="3:9" ht="12.95" customHeight="1">
       <c r="C24" s="3"/>
       <c r="D24" s="33" t="s">
-        <v>219</v>
+        <v>332</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
@@ -9744,7 +9811,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="64"/>
     </row>
-    <row r="25" spans="3:9" ht="13" customHeight="1">
+    <row r="25" spans="3:9" ht="12.95" customHeight="1">
       <c r="C25" s="17"/>
       <c r="D25" s="49" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
committing userstory 25 testcases and updated excel sheet -uploading on behalf of Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens\Courses\CS-555-Agile Methods for SW Eng\GEDCOMProject\CS_555_JAVS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shree\Downloads\Semester 2\Agile\GedcomProject\CS_555_JAVS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0290669-7099-4AB2-B4D6-AF4AF484DBCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F03E3AF6-2B78-4D58-AD08-944DDE49A984}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9850" yWindow="1820" windowWidth="28800" windowHeight="15460" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="Sprint4" sheetId="9" r:id="rId9"/>
     <sheet name="Stories" sheetId="10" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Backlog!$A$1:$E$33</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="346">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -339,9 +342,6 @@
     <t>Marriage before divorce</t>
   </si>
   <si>
-    <t xml:space="preserve">           3</t>
-  </si>
-  <si>
     <t>US06</t>
   </si>
   <si>
@@ -1115,7 +1115,49 @@
     <t>347-409</t>
   </si>
   <si>
-    <t>Avoid inegration at the end, Avoid editing other US's test data in gedcom file-create your own test data</t>
+    <t>US25_Unique_Names_BirthDate</t>
+  </si>
+  <si>
+    <t>12-51</t>
+  </si>
+  <si>
+    <t>Test_US25_UniqueNamesBirthdate</t>
+  </si>
+  <si>
+    <t>testUniqueNamesBirthdate, testUniqueNamesBirthdate2</t>
+  </si>
+  <si>
+    <t>13-75</t>
+  </si>
+  <si>
+    <t>US_Unique_Names.java</t>
+  </si>
+  <si>
+    <t>listOfUpcoming_Anniversaries</t>
+  </si>
+  <si>
+    <t>36-65</t>
+  </si>
+  <si>
+    <t>Test_CheckList.java</t>
+  </si>
+  <si>
+    <t>test_Check_LivingMarried_Upcomming_Anniversary, test_Check_LivingMarried_Upcomming_Anniversary2</t>
+  </si>
+  <si>
+    <t>227-281</t>
+  </si>
+  <si>
+    <t>Completion of User stories on time</t>
+  </si>
+  <si>
+    <t>Writing Test Cases on time</t>
+  </si>
+  <si>
+    <t>Avoid late completion of user stories</t>
+  </si>
+  <si>
+    <t>Anser ASAP on slack messages</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1514,6 +1556,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1923,6 +1966,9 @@
                 <c:pt idx="3" formatCode="m/d/yyyy">
                   <c:v>42101</c:v>
                 </c:pt>
+                <c:pt idx="4" formatCode="m/d/yyyy">
+                  <c:v>42115</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1943,6 +1989,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2160,8 +2209,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1220487" y="1267638"/>
-          <a:ext cx="1446994" cy="1044549"/>
+          <a:off x="1287162" y="1289863"/>
+          <a:ext cx="1504144" cy="1066774"/>
           <a:chOff x="-19049" y="-41148"/>
           <a:chExt cx="1446994" cy="1066774"/>
         </a:xfrm>
@@ -2296,7 +2345,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2430,8 +2479,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5209322" y="1286736"/>
-          <a:ext cx="1367161" cy="776329"/>
+          <a:off x="5625247" y="1308961"/>
+          <a:ext cx="1433836" cy="792204"/>
           <a:chOff x="-19051" y="-41148"/>
           <a:chExt cx="1363986" cy="792204"/>
         </a:xfrm>
@@ -2566,7 +2615,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2653,8 +2702,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2715893" y="1071427"/>
-          <a:ext cx="1174540" cy="1055700"/>
+          <a:off x="2839718" y="1090477"/>
+          <a:ext cx="1349165" cy="1077925"/>
           <a:chOff x="-19050" y="-52578"/>
           <a:chExt cx="1177716" cy="1077924"/>
         </a:xfrm>
@@ -2789,7 +2838,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2876,8 +2925,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3743294" y="1426511"/>
-          <a:ext cx="538509" cy="654002"/>
+          <a:off x="4041744" y="1451911"/>
+          <a:ext cx="579784" cy="666702"/>
           <a:chOff x="-19050" y="-31618"/>
           <a:chExt cx="535334" cy="666701"/>
         </a:xfrm>
@@ -3012,7 +3061,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3146,8 +3195,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4160517" y="1092593"/>
-          <a:ext cx="1235924" cy="1111242"/>
+          <a:off x="4458967" y="1111643"/>
+          <a:ext cx="1353399" cy="1133467"/>
           <a:chOff x="-19050" y="-52578"/>
           <a:chExt cx="1232748" cy="1133467"/>
         </a:xfrm>
@@ -3282,7 +3331,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3369,8 +3418,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5362048" y="4857553"/>
-          <a:ext cx="1341754" cy="973698"/>
+          <a:off x="5777973" y="4949628"/>
+          <a:ext cx="1408429" cy="995923"/>
           <a:chOff x="-19051" y="-41148"/>
           <a:chExt cx="1338579" cy="995923"/>
         </a:xfrm>
@@ -3505,7 +3554,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -4721,10 +4770,10 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.75" customWidth="1"/>
+    <col min="2" max="4" width="33.765625" customWidth="1"/>
     <col min="5" max="256" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4792,7 +4841,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="15.95" customHeight="1">
+    <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
         <v>4</v>
@@ -4801,7 +4850,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="15.95" customHeight="1">
+    <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
@@ -4812,7 +4861,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="15.95" customHeight="1">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -4821,7 +4870,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="15.95" customHeight="1">
+    <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -4832,7 +4881,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="15.95" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
         <v>9</v>
@@ -4841,7 +4890,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="15.95" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -4852,7 +4901,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -4861,7 +4910,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="15.95" customHeight="1">
+    <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
@@ -4872,7 +4921,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="15.95" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -4881,7 +4930,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="15.95" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
@@ -4892,7 +4941,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="15.95" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
@@ -4901,7 +4950,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="15.95" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
@@ -4912,7 +4961,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15.95" customHeight="1">
+    <row r="21" spans="1:5" ht="16" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="8" t="s">
         <v>17</v>
@@ -4921,7 +4970,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="15.95" customHeight="1">
+    <row r="22" spans="1:5" ht="16" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11" t="s">
@@ -4932,7 +4981,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="15.95" customHeight="1">
+    <row r="23" spans="1:5" ht="16" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" s="8" t="s">
         <v>19</v>
@@ -4941,7 +4990,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="15.95" customHeight="1">
+    <row r="24" spans="1:5" ht="16" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
@@ -4952,7 +5001,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="15.95" customHeight="1">
+    <row r="25" spans="1:5" ht="16" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="8" t="s">
         <v>21</v>
@@ -4961,7 +5010,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="15.95" customHeight="1">
+    <row r="26" spans="1:5" ht="16" customHeight="1">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
@@ -4992,12 +5041,12 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="28.125" customWidth="1"/>
-    <col min="3" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="256" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" customWidth="1"/>
+    <col min="4" max="256" width="10.84375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">
@@ -5008,12 +5057,12 @@
         <v>52</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="2" spans="1:5" ht="34" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>64</v>
       </c>
@@ -5021,7 +5070,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -5034,7 +5083,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -5047,12 +5096,12 @@
         <v>59</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="5" spans="1:5" ht="34" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>72</v>
       </c>
@@ -5060,7 +5109,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -5073,20 +5122,20 @@
         <v>69</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" ht="17.25" customHeight="1">
       <c r="A7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>76</v>
-      </c>
       <c r="C7" s="63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -5099,12 +5148,12 @@
         <v>61</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="9" spans="1:5" ht="34" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>70</v>
       </c>
@@ -5112,25 +5161,25 @@
         <v>71</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="10" spans="1:5" ht="34" customHeight="1">
       <c r="A10" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>78</v>
-      </c>
       <c r="C10" s="63" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="11" spans="1:5" ht="34" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>62</v>
       </c>
@@ -5138,12 +5187,12 @@
         <v>63</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="12" spans="1:5" ht="34" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>66</v>
       </c>
@@ -5151,410 +5200,410 @@
         <v>67</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="51" customHeight="1">
       <c r="A13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="C13" s="63" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" ht="68.25" customHeight="1">
       <c r="A14" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="C14" s="63" t="s">
         <v>279</v>
-      </c>
-      <c r="C14" s="63" t="s">
-        <v>280</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="15" spans="1:5" ht="34" customHeight="1">
       <c r="A15" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>82</v>
-      </c>
       <c r="C15" s="63" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" ht="17.25" customHeight="1">
       <c r="A16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>84</v>
-      </c>
       <c r="C16" s="63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
     </row>
-    <row r="17" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="17" spans="1:5" ht="34" customHeight="1">
       <c r="A17" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>86</v>
-      </c>
       <c r="C17" s="63" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" ht="17.25" customHeight="1">
       <c r="A18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="C18" s="63" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1">
       <c r="A19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="C19" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" ht="17.25" customHeight="1">
       <c r="A20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>93</v>
-      </c>
       <c r="C20" s="63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="21" spans="1:5" ht="34" customHeight="1">
       <c r="A21" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>95</v>
-      </c>
       <c r="C21" s="63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="22" spans="1:5" ht="34" customHeight="1">
       <c r="A22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="C22" s="63" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="23" spans="1:5" ht="34" customHeight="1">
       <c r="A23" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>99</v>
-      </c>
       <c r="C23" s="63" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="24" spans="1:5" ht="34" customHeight="1">
       <c r="A24" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>101</v>
-      </c>
       <c r="C24" s="63" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" ht="51" customHeight="1">
       <c r="A25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>103</v>
-      </c>
       <c r="C25" s="63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="26" spans="1:5" ht="34" customHeight="1">
       <c r="A26" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="C26" s="63" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="135.94999999999999" customHeight="1">
+    <row r="27" spans="1:5" ht="136" customHeight="1">
       <c r="A27" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="C27" s="63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" ht="17.25" customHeight="1">
       <c r="A28" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="C28" s="63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="29" spans="1:5" ht="34" customHeight="1">
       <c r="A29" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>111</v>
-      </c>
       <c r="C29" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="17.25" customHeight="1">
       <c r="A30" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="C30" s="63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="17.25" customHeight="1">
       <c r="A31" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>115</v>
-      </c>
       <c r="C31" s="63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="32" spans="1:5" ht="34" customHeight="1">
       <c r="A32" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>117</v>
-      </c>
       <c r="C32" s="63" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5" ht="17.25" customHeight="1">
       <c r="A33" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="C33" s="63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
     </row>
-    <row r="34" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="34" spans="1:5" ht="34" customHeight="1">
       <c r="A34" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="C34" s="63" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" ht="51" customHeight="1">
       <c r="A35" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>128</v>
-      </c>
       <c r="C35" s="63" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="36" spans="1:5" ht="34" customHeight="1">
       <c r="A36" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>123</v>
-      </c>
       <c r="C36" s="63" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="37" spans="1:5" ht="34" customHeight="1">
       <c r="A37" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="C37" s="63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="38" spans="1:5" ht="34" customHeight="1">
       <c r="A38" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="C38" s="63" t="s">
         <v>304</v>
-      </c>
-      <c r="C38" s="63" t="s">
-        <v>305</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="39" spans="1:5" ht="34" customHeight="1">
       <c r="A39" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>130</v>
-      </c>
       <c r="C39" s="63" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="40" spans="1:5" ht="34" customHeight="1">
       <c r="A40" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="C40" s="63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="41" spans="1:5" ht="34" customHeight="1">
       <c r="A41" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="C41" s="63" t="s">
         <v>309</v>
-      </c>
-      <c r="C41" s="63" t="s">
-        <v>310</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="42" spans="1:5" ht="34" customHeight="1">
       <c r="A42" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="C42" s="63" t="s">
         <v>312</v>
-      </c>
-      <c r="C42" s="63" t="s">
-        <v>313</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="43" spans="1:5" ht="34" customHeight="1">
       <c r="A43" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="C43" s="63" t="s">
         <v>315</v>
-      </c>
-      <c r="C43" s="63" t="s">
-        <v>316</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
@@ -5576,10 +5625,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" customWidth="1"/>
+    <col min="2" max="2" width="10.765625" customWidth="1"/>
+    <col min="3" max="3" width="10.84375" customWidth="1"/>
+    <col min="4" max="5" width="20.4609375" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5718,19 +5767,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="25.25" customWidth="1"/>
-    <col min="4" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="8.15234375" customWidth="1"/>
+    <col min="2" max="2" width="7.765625" customWidth="1"/>
+    <col min="3" max="3" width="25.23046875" customWidth="1"/>
+    <col min="4" max="4" width="6.765625" customWidth="1"/>
+    <col min="5" max="5" width="7.765625" customWidth="1"/>
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5905,14 +5954,14 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="67">
+        <v>3</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>33</v>
@@ -5922,14 +5971,14 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="18" t="s">
-        <v>74</v>
+      <c r="A12" s="67">
+        <v>3</v>
       </c>
       <c r="B12" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>28</v>
@@ -5939,14 +5988,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="19">
+      <c r="A13" s="67">
         <v>2</v>
       </c>
       <c r="B13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>33</v>
@@ -5956,14 +6005,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="18" t="s">
-        <v>74</v>
+      <c r="A14" s="67">
+        <v>3</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>33</v>
@@ -5977,10 +6026,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>28</v>
@@ -5994,16 +6043,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
@@ -6011,10 +6060,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>33</v>
@@ -6028,10 +6077,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>38</v>
@@ -6042,59 +6091,67 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+        <v>96</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+        <v>98</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>57</v>
@@ -6105,16 +6162,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
@@ -6122,13 +6179,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>57</v>
@@ -6136,231 +6193,159 @@
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+        <v>114</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="19">
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="19">
+        <v>3</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1">
+      <c r="A29" s="23">
         <v>4</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="19">
-        <v>2</v>
-      </c>
       <c r="B29" s="18" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="23">
+        <v>4</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A31" s="24">
+        <v>4</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E31" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="19">
-        <v>3</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="18" t="s">
+    <row r="32" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A32" s="27">
+        <v>4</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A33" s="30">
+        <v>4</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E33" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="19">
-        <v>4</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1">
-      <c r="A32" s="19">
-        <v>4</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-    </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A33" s="19">
-        <v>3</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="21" customHeight="1">
-      <c r="A34" s="23">
-        <v>4</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="23">
-        <v>4</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A36" s="24">
-        <v>4</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A37" s="27">
-        <v>4</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A38" s="30">
-        <v>4</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:E33" xr:uid="{20A94F15-62DA-4524-8A28-DF027B8E04DC}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -6375,20 +6360,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" customWidth="1"/>
+    <col min="7" max="256" width="10.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.95" customHeight="1">
+    <row r="1" spans="1:8" ht="13" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -6398,9 +6383,9 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" ht="12.95" customHeight="1">
+    <row r="2" spans="1:8" ht="13" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -6410,9 +6395,9 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
-    <row r="3" spans="1:8" ht="12.95" customHeight="1">
+    <row r="3" spans="1:8" ht="13" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -6422,7 +6407,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:8" ht="12.95" customHeight="1">
+    <row r="4" spans="1:8" ht="13" customHeight="1">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -6432,9 +6417,9 @@
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:8" ht="12.95" customHeight="1">
+    <row r="5" spans="1:8" ht="13" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -6444,9 +6429,9 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="12.95" customHeight="1">
+    <row r="6" spans="1:8" ht="13" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -6456,7 +6441,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" ht="12.95" customHeight="1">
+    <row r="7" spans="1:8" ht="13" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -6466,9 +6451,9 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:8" ht="12.95" customHeight="1">
+    <row r="8" spans="1:8" ht="13" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -6478,7 +6463,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
     </row>
-    <row r="9" spans="1:8" ht="12.95" customHeight="1">
+    <row r="9" spans="1:8" ht="13" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -6488,7 +6473,7 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="1:8" ht="12.95" customHeight="1">
+    <row r="10" spans="1:8" ht="13" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -6498,7 +6483,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:8" ht="12.95" customHeight="1">
+    <row r="11" spans="1:8" ht="13" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -6508,7 +6493,7 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" spans="1:8" ht="12.95" customHeight="1">
+    <row r="12" spans="1:8" ht="13" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -6518,7 +6503,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" ht="12.95" customHeight="1">
+    <row r="13" spans="1:8" ht="13" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -6528,33 +6513,33 @@
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" ht="12.95" customHeight="1">
+    <row r="14" spans="1:8" ht="13" customHeight="1">
       <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="D14" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="E14" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="F14" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="G14" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:8" ht="13" customHeight="1">
+      <c r="A15" s="18" t="s">
         <v>144</v>
-      </c>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" ht="12.95" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>145</v>
       </c>
       <c r="B15" s="34">
         <v>42046</v>
@@ -6570,9 +6555,9 @@
       <c r="G15" s="37"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="12.95" customHeight="1">
+    <row r="16" spans="1:8" ht="13" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="34">
         <v>42060</v>
@@ -6596,9 +6581,9 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="12.95" customHeight="1">
+    <row r="17" spans="1:8" ht="13" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" s="34">
         <v>42087</v>
@@ -6622,9 +6607,9 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="12.95" customHeight="1">
+    <row r="18" spans="1:8" ht="13" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B18" s="34">
         <v>42101</v>
@@ -6648,9 +6633,9 @@
       </c>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="12.95" customHeight="1">
+    <row r="19" spans="1:8" ht="13" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="35">
@@ -6672,7 +6657,7 @@
       </c>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="12.95" customHeight="1">
+    <row r="20" spans="1:8" ht="13" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="30"/>
@@ -6682,7 +6667,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="12.95" customHeight="1">
+    <row r="21" spans="1:8" ht="13" customHeight="1">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -6692,7 +6677,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="12.95" customHeight="1">
+    <row r="22" spans="1:8" ht="13" customHeight="1">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -6702,7 +6687,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="12.95" customHeight="1">
+    <row r="23" spans="1:8" ht="13" customHeight="1">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -6712,7 +6697,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" ht="12.95" customHeight="1">
+    <row r="24" spans="1:8" ht="13" customHeight="1">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -6722,7 +6707,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" ht="12.95" customHeight="1">
+    <row r="25" spans="1:8" ht="13" customHeight="1">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -6732,7 +6717,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="12.95" customHeight="1">
+    <row r="26" spans="1:8" ht="13" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -6742,7 +6727,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="12.95" customHeight="1">
+    <row r="27" spans="1:8" ht="13" customHeight="1">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -6752,7 +6737,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="1:8" ht="12.95" customHeight="1">
+    <row r="28" spans="1:8" ht="13" customHeight="1">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -6762,7 +6747,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="1:8" ht="12.95" customHeight="1">
+    <row r="29" spans="1:8" ht="13" customHeight="1">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -6772,7 +6757,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="12.95" customHeight="1">
+    <row r="30" spans="1:8" ht="13" customHeight="1">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -6782,7 +6767,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="12.95" customHeight="1">
+    <row r="31" spans="1:8" ht="13" customHeight="1">
       <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -6792,7 +6777,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="1:8" ht="12.95" customHeight="1">
+    <row r="32" spans="1:8" ht="13" customHeight="1">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -6802,7 +6787,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="12.95" customHeight="1">
+    <row r="33" spans="1:8" ht="13" customHeight="1">
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -6812,7 +6797,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
     </row>
-    <row r="34" spans="1:8" ht="12.95" customHeight="1">
+    <row r="34" spans="1:8" ht="13" customHeight="1">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -6822,7 +6807,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:8" ht="12.95" customHeight="1">
+    <row r="35" spans="1:8" ht="13" customHeight="1">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -6832,7 +6817,7 @@
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8" ht="12.95" customHeight="1">
+    <row r="36" spans="1:8" ht="13" customHeight="1">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
@@ -6842,7 +6827,7 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
     </row>
-    <row r="37" spans="1:8" ht="12.95" customHeight="1">
+    <row r="37" spans="1:8" ht="13" customHeight="1">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -6852,7 +6837,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8" ht="12.95" customHeight="1">
+    <row r="38" spans="1:8" ht="13" customHeight="1">
       <c r="A38" s="19"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -6862,7 +6847,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="12.95" customHeight="1">
+    <row r="39" spans="1:8" ht="13" customHeight="1">
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -6886,43 +6871,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="256" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" customWidth="1"/>
+    <col min="2" max="2" width="16.765625" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" customWidth="1"/>
+    <col min="7" max="256" width="10.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.95" customHeight="1">
+    <row r="1" spans="1:7" ht="13" customHeight="1">
       <c r="A1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>144</v>
-      </c>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" ht="12.95" customHeight="1">
+    <row r="2" spans="1:7" ht="13" customHeight="1">
       <c r="A2" s="39">
         <v>42046</v>
       </c>
@@ -6937,7 +6922,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="12.95" customHeight="1">
+    <row r="3" spans="1:7" ht="13" customHeight="1">
       <c r="A3" s="39">
         <v>42059</v>
       </c>
@@ -6960,7 +6945,7 @@
       </c>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="12.95" customHeight="1">
+    <row r="4" spans="1:7" ht="13" customHeight="1">
       <c r="A4" s="41">
         <v>42087</v>
       </c>
@@ -6981,7 +6966,7 @@
       </c>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="12.95" customHeight="1">
+    <row r="5" spans="1:7" ht="13" customHeight="1">
       <c r="A5" s="41">
         <v>42101</v>
       </c>
@@ -7002,16 +6987,22 @@
       </c>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="12.95" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+    <row r="6" spans="1:7" ht="13" customHeight="1">
+      <c r="A6" s="41">
+        <v>42115</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0</v>
+      </c>
+      <c r="C6" s="19">
+        <v>8</v>
+      </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="12.95" customHeight="1">
+    <row r="7" spans="1:7" ht="13" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -7020,7 +7011,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="12.95" customHeight="1">
+    <row r="8" spans="1:7" ht="13" customHeight="1">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -7029,7 +7020,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="12.95" customHeight="1">
+    <row r="9" spans="1:7" ht="13" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -7038,7 +7029,7 @@
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7" ht="12.95" customHeight="1">
+    <row r="10" spans="1:7" ht="13" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -7047,7 +7038,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" ht="12.95" customHeight="1">
+    <row r="11" spans="1:7" ht="13" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -7056,7 +7047,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7" ht="12.95" customHeight="1">
+    <row r="12" spans="1:7" ht="13" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -7065,7 +7056,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:7" ht="12.95" customHeight="1">
+    <row r="13" spans="1:7" ht="13" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -7074,7 +7065,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:7" ht="12.95" customHeight="1">
+    <row r="14" spans="1:7" ht="13" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -7083,7 +7074,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" ht="12.95" customHeight="1">
+    <row r="15" spans="1:7" ht="13" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -7092,7 +7083,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:7" ht="12.95" customHeight="1">
+    <row r="16" spans="1:7" ht="13" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -7101,7 +7092,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="1:7" ht="12.95" customHeight="1">
+    <row r="17" spans="1:7" ht="13" customHeight="1">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -7110,7 +7101,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" ht="12.95" customHeight="1">
+    <row r="18" spans="1:7" ht="13" customHeight="1">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -7119,7 +7110,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" ht="12.95" customHeight="1">
+    <row r="19" spans="1:7" ht="13" customHeight="1">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -7128,7 +7119,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="12.95" customHeight="1">
+    <row r="20" spans="1:7" ht="13" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -7137,7 +7128,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="12.95" customHeight="1">
+    <row r="21" spans="1:7" ht="13" customHeight="1">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -7146,7 +7137,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="12.95" customHeight="1">
+    <row r="22" spans="1:7" ht="13" customHeight="1">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -7155,7 +7146,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
     </row>
-    <row r="23" spans="1:7" ht="12.95" customHeight="1">
+    <row r="23" spans="1:7" ht="13" customHeight="1">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -7164,7 +7155,7 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="12.95" customHeight="1">
+    <row r="24" spans="1:7" ht="13" customHeight="1">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -7173,7 +7164,7 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="12.95" customHeight="1">
+    <row r="25" spans="1:7" ht="13" customHeight="1">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -7182,7 +7173,7 @@
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="12.95" customHeight="1">
+    <row r="26" spans="1:7" ht="13" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -7209,22 +7200,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.75" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="7.25" customWidth="1"/>
-    <col min="4" max="4" width="8.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
+    <col min="1" max="1" width="7.765625" customWidth="1"/>
+    <col min="2" max="2" width="24.4609375" customWidth="1"/>
+    <col min="3" max="3" width="7.23046875" customWidth="1"/>
+    <col min="4" max="4" width="8.23046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" customWidth="1"/>
+    <col min="7" max="7" width="8.4609375" customWidth="1"/>
+    <col min="8" max="8" width="9.23046875" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="19.125" customWidth="1"/>
+    <col min="11" max="11" width="11.4609375" customWidth="1"/>
+    <col min="12" max="12" width="19.15234375" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="1.875" customWidth="1"/>
-    <col min="15" max="15" width="10.125" customWidth="1"/>
-    <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="10.125" customWidth="1"/>
+    <col min="14" max="14" width="1.84375" customWidth="1"/>
+    <col min="15" max="15" width="10.15234375" customWidth="1"/>
+    <col min="16" max="16" width="16.4609375" customWidth="1"/>
+    <col min="17" max="17" width="10.15234375" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7242,39 +7233,39 @@
         <v>54</v>
       </c>
       <c r="E1" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="G1" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="43" t="s">
         <v>152</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>153</v>
       </c>
       <c r="I1" s="43" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>155</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>156</v>
       </c>
       <c r="N1" s="19"/>
       <c r="O1" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="P1" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="Q1" s="44" t="s">
         <v>158</v>
-      </c>
-      <c r="Q1" s="44" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1">
@@ -7288,7 +7279,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E2" s="19">
         <v>100</v>
@@ -7303,24 +7294,24 @@
         <v>45</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="M2" s="18" t="s">
         <v>163</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>164</v>
       </c>
       <c r="N2" s="19"/>
       <c r="O2" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>166</v>
       </c>
       <c r="Q2" s="19">
         <v>113</v>
@@ -7337,7 +7328,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="19">
         <v>100</v>
@@ -7352,24 +7343,24 @@
         <v>25</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L3" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q3" s="19">
         <v>20</v>
@@ -7386,7 +7377,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="19">
         <v>102</v>
@@ -7401,24 +7392,24 @@
         <v>100</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="L4" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>171</v>
       </c>
       <c r="M4" s="46">
         <v>48944</v>
       </c>
       <c r="N4" s="19"/>
       <c r="O4" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" s="45" t="s">
         <v>172</v>
-      </c>
-      <c r="P4" s="45" t="s">
-        <v>173</v>
       </c>
       <c r="Q4" s="19">
         <v>8</v>
@@ -7435,7 +7426,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="19">
         <v>100</v>
@@ -7450,24 +7441,24 @@
         <v>50</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>174</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>175</v>
       </c>
       <c r="N5" s="19"/>
       <c r="O5" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P5" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q5" s="19">
         <v>11</v>
@@ -7484,7 +7475,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" s="19">
         <v>90</v>
@@ -7499,24 +7490,24 @@
         <v>30</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="L6" s="45" t="s">
+      <c r="M6" s="18" t="s">
         <v>178</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>179</v>
       </c>
       <c r="N6" s="19"/>
       <c r="O6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="45" t="s">
         <v>180</v>
-      </c>
-      <c r="P6" s="45" t="s">
-        <v>181</v>
       </c>
       <c r="Q6" s="19">
         <v>232</v>
@@ -7533,7 +7524,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E7" s="19">
         <v>100</v>
@@ -7548,24 +7539,24 @@
         <v>180</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L7" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7" s="18" t="s">
         <v>182</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>183</v>
       </c>
       <c r="N7" s="19"/>
       <c r="O7" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q7" s="19">
         <v>43</v>
@@ -7582,7 +7573,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8" s="19">
         <v>105</v>
@@ -7597,24 +7588,24 @@
         <v>75</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L8" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M8" s="46">
         <v>51470</v>
       </c>
       <c r="N8" s="19"/>
       <c r="O8" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="P8" s="45" t="s">
         <v>186</v>
-      </c>
-      <c r="P8" s="45" t="s">
-        <v>187</v>
       </c>
       <c r="Q8" s="19">
         <v>182</v>
@@ -7631,7 +7622,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E9" s="19">
         <v>100</v>
@@ -7646,24 +7637,24 @@
         <v>60</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L9" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>189</v>
       </c>
       <c r="N9" s="19"/>
       <c r="O9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="P9" s="45" t="s">
         <v>190</v>
-      </c>
-      <c r="P9" s="45" t="s">
-        <v>191</v>
       </c>
       <c r="Q9" s="19">
         <v>167</v>
@@ -7748,7 +7739,7 @@
     <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -7788,10 +7779,10 @@
     <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>193</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>194</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -7812,7 +7803,7 @@
       <c r="A17" s="19"/>
       <c r="B17" s="47"/>
       <c r="C17" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -7833,7 +7824,7 @@
       <c r="A18" s="19"/>
       <c r="B18" s="47"/>
       <c r="C18" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -7872,10 +7863,10 @@
     <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>197</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>198</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
@@ -7910,12 +7901,12 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="20.765625" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="22.75" customWidth="1"/>
+    <col min="12" max="12" width="22.765625" customWidth="1"/>
     <col min="13" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="19.25" customWidth="1"/>
-    <col min="16" max="16" width="190.75" customWidth="1"/>
+    <col min="15" max="15" width="19.23046875" customWidth="1"/>
+    <col min="16" max="16" width="190.765625" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="256" width="11" customWidth="1"/>
   </cols>
@@ -7934,53 +7925,53 @@
         <v>54</v>
       </c>
       <c r="E1" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="G1" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="43" t="s">
         <v>152</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>153</v>
       </c>
       <c r="I1" s="43" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="24"/>
       <c r="K1" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>155</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>156</v>
       </c>
       <c r="N1" s="19"/>
       <c r="O1" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="P1" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="Q1" s="44" t="s">
         <v>158</v>
-      </c>
-      <c r="Q1" s="44" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="A2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>97</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="19">
         <v>115</v>
@@ -7995,24 +7986,24 @@
         <v>25</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L2" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="M2" s="18" t="s">
         <v>200</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>201</v>
       </c>
       <c r="N2" s="19"/>
       <c r="O2" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>203</v>
       </c>
       <c r="Q2" s="19">
         <v>85</v>
@@ -8020,16 +8011,16 @@
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="A3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>99</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" s="19">
         <v>100</v>
@@ -8044,24 +8035,24 @@
         <v>35</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="L3" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="M3" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>207</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>208</v>
       </c>
       <c r="Q3" s="19">
         <v>68</v>
@@ -8069,16 +8060,16 @@
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="A4" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="19">
         <v>80</v>
@@ -8093,24 +8084,24 @@
         <v>15</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J4" s="27"/>
       <c r="K4" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="L4" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>171</v>
       </c>
       <c r="M4" s="46">
         <v>48944</v>
       </c>
       <c r="N4" s="19"/>
       <c r="O4" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" s="45" t="s">
         <v>172</v>
-      </c>
-      <c r="P4" s="45" t="s">
-        <v>173</v>
       </c>
       <c r="Q4" s="19">
         <v>8</v>
@@ -8127,7 +8118,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="19">
         <v>100</v>
@@ -8142,24 +8133,24 @@
         <v>20</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J5" s="27"/>
       <c r="K5" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>174</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>175</v>
       </c>
       <c r="N5" s="19"/>
       <c r="O5" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P5" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q5" s="19">
         <v>11</v>
@@ -8167,16 +8158,16 @@
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="A6" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="19">
         <v>90</v>
@@ -8191,24 +8182,24 @@
         <v>20</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J6" s="27"/>
       <c r="K6" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L6" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" s="18" t="s">
         <v>209</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>210</v>
       </c>
       <c r="N6" s="19"/>
       <c r="O6" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="P6" s="45" t="s">
         <v>211</v>
-      </c>
-      <c r="P6" s="45" t="s">
-        <v>212</v>
       </c>
       <c r="Q6" s="19">
         <v>232</v>
@@ -8216,16 +8207,16 @@
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1">
       <c r="A7" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>113</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="19">
         <v>95</v>
@@ -8240,24 +8231,24 @@
         <v>10</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L7" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="M7" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>214</v>
       </c>
       <c r="N7" s="19"/>
       <c r="O7" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q7" s="19">
         <v>43</v>
@@ -8265,16 +8256,16 @@
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1">
       <c r="A8" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="19">
         <v>98</v>
@@ -8289,24 +8280,24 @@
         <v>90</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L8" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M8" s="46">
         <v>51470</v>
       </c>
       <c r="N8" s="19"/>
       <c r="O8" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="P8" s="45" t="s">
         <v>186</v>
-      </c>
-      <c r="P8" s="45" t="s">
-        <v>187</v>
       </c>
       <c r="Q8" s="19">
         <v>182</v>
@@ -8314,16 +8305,16 @@
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="19">
         <v>105</v>
@@ -8338,24 +8329,24 @@
         <v>90</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L9" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>189</v>
       </c>
       <c r="N9" s="19"/>
       <c r="O9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="P9" s="45" t="s">
         <v>190</v>
-      </c>
-      <c r="P9" s="45" t="s">
-        <v>191</v>
       </c>
       <c r="Q9" s="19">
         <v>167</v>
@@ -8421,7 +8412,7 @@
     <row r="13" spans="1:17" ht="14.25" customHeight="1">
       <c r="A13" s="27"/>
       <c r="B13" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -8461,10 +8452,10 @@
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
       <c r="A15" s="27"/>
       <c r="B15" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -8485,7 +8476,7 @@
       <c r="A16" s="27"/>
       <c r="B16" s="47"/>
       <c r="C16" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -8543,10 +8534,10 @@
     <row r="19" spans="1:17" ht="14.25" customHeight="1">
       <c r="A19" s="27"/>
       <c r="B19" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -8567,7 +8558,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
@@ -8588,7 +8579,7 @@
       <c r="A21" s="13"/>
       <c r="B21" s="17"/>
       <c r="C21" s="49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="48"/>
@@ -8625,9 +8616,9 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="22.765625" customWidth="1"/>
     <col min="3" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="20.4609375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="256" width="11" customWidth="1"/>
   </cols>
@@ -8646,52 +8637,52 @@
         <v>54</v>
       </c>
       <c r="E1" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>152</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>153</v>
       </c>
       <c r="I1" s="51" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="L1" s="52" t="s">
         <v>155</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>156</v>
       </c>
       <c r="M1" s="53"/>
       <c r="N1" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="P1" s="52" t="s">
         <v>158</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
       <c r="A2" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>78</v>
-      </c>
       <c r="C2" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>221</v>
-      </c>
-      <c r="D2" s="54" t="s">
-        <v>222</v>
       </c>
       <c r="E2" s="53">
         <v>50</v>
@@ -8706,23 +8697,23 @@
         <v>30</v>
       </c>
       <c r="I2" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J2" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="L2" s="54" t="s">
         <v>224</v>
-      </c>
-      <c r="L2" s="54" t="s">
-        <v>225</v>
       </c>
       <c r="M2" s="53"/>
       <c r="N2" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" s="54" t="s">
         <v>226</v>
-      </c>
-      <c r="O2" s="54" t="s">
-        <v>227</v>
       </c>
       <c r="P2" s="55">
         <v>236</v>
@@ -8730,16 +8721,16 @@
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>103</v>
-      </c>
       <c r="C3" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>221</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>222</v>
       </c>
       <c r="E3" s="53">
         <v>50</v>
@@ -8754,23 +8745,23 @@
         <v>30</v>
       </c>
       <c r="I3" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J3" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="K3" s="54" t="s">
         <v>228</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="L3" s="54" t="s">
         <v>229</v>
-      </c>
-      <c r="L3" s="54" t="s">
-        <v>230</v>
       </c>
       <c r="M3" s="53"/>
       <c r="N3" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="O3" s="54" t="s">
         <v>231</v>
-      </c>
-      <c r="O3" s="54" t="s">
-        <v>232</v>
       </c>
       <c r="P3" s="55">
         <v>96</v>
@@ -8778,16 +8769,16 @@
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>82</v>
-      </c>
       <c r="C4" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E4" s="53">
         <v>70</v>
@@ -8802,23 +8793,23 @@
         <v>90</v>
       </c>
       <c r="I4" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J4" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="K4" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="L4" s="54" t="s">
         <v>235</v>
-      </c>
-      <c r="L4" s="54" t="s">
-        <v>236</v>
       </c>
       <c r="M4" s="53"/>
       <c r="N4" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="O4" s="57" t="s">
         <v>237</v>
-      </c>
-      <c r="O4" s="57" t="s">
-        <v>238</v>
       </c>
       <c r="P4" s="55">
         <v>50</v>
@@ -8826,16 +8817,16 @@
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="A5" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>76</v>
-      </c>
       <c r="C5" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" s="53">
         <v>50</v>
@@ -8850,23 +8841,23 @@
         <v>90</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K5" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="L5" s="54" t="s">
         <v>239</v>
-      </c>
-      <c r="L5" s="54" t="s">
-        <v>240</v>
       </c>
       <c r="M5" s="53"/>
       <c r="N5" s="54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O5" s="57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P5" s="55">
         <v>26</v>
@@ -8874,16 +8865,16 @@
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1">
       <c r="A6" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="54" t="s">
         <v>116</v>
-      </c>
-      <c r="B6" s="54" t="s">
-        <v>117</v>
       </c>
       <c r="C6" s="54" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="53">
         <v>50</v>
@@ -8898,23 +8889,23 @@
         <v>30</v>
       </c>
       <c r="I6" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J6" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="K6" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="L6" s="54" t="s">
         <v>243</v>
-      </c>
-      <c r="L6" s="54" t="s">
-        <v>244</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54" t="s">
+        <v>244</v>
+      </c>
+      <c r="O6" s="57" t="s">
         <v>245</v>
-      </c>
-      <c r="O6" s="57" t="s">
-        <v>246</v>
       </c>
       <c r="P6" s="55">
         <v>34</v>
@@ -8922,16 +8913,16 @@
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>120</v>
-      </c>
-      <c r="B7" s="54" t="s">
-        <v>121</v>
       </c>
       <c r="C7" s="54" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E7" s="53">
         <v>50</v>
@@ -8946,23 +8937,23 @@
         <v>15</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="L7" s="54" t="s">
         <v>247</v>
-      </c>
-      <c r="L7" s="54" t="s">
-        <v>248</v>
       </c>
       <c r="M7" s="53"/>
       <c r="N7" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P7" s="55">
         <v>34</v>
@@ -8970,16 +8961,16 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="54" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" s="53">
         <v>60</v>
@@ -8994,23 +8985,23 @@
         <v>20</v>
       </c>
       <c r="I8" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J8" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="K8" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="K8" s="56" t="s">
+      <c r="L8" s="54" t="s">
         <v>252</v>
-      </c>
-      <c r="L8" s="54" t="s">
-        <v>253</v>
       </c>
       <c r="M8" s="53"/>
       <c r="N8" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P8" s="55">
         <v>14</v>
@@ -9018,16 +9009,16 @@
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="A9" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" s="54" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9" s="53">
         <v>65</v>
@@ -9042,23 +9033,23 @@
         <v>20</v>
       </c>
       <c r="I9" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K9" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="L9" s="54" t="s">
         <v>256</v>
-      </c>
-      <c r="L9" s="54" t="s">
-        <v>257</v>
       </c>
       <c r="M9" s="53"/>
       <c r="N9" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P9" s="55">
         <v>67</v>
@@ -9157,7 +9148,7 @@
     <row r="15" spans="1:16" ht="14.25" customHeight="1">
       <c r="A15" s="27"/>
       <c r="B15" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -9195,10 +9186,10 @@
     <row r="17" spans="1:16" ht="14.25" customHeight="1">
       <c r="A17" s="27"/>
       <c r="B17" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -9218,7 +9209,7 @@
       <c r="A18" s="27"/>
       <c r="B18" s="47"/>
       <c r="C18" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -9273,10 +9264,10 @@
     <row r="21" spans="1:16" ht="14.25" customHeight="1">
       <c r="A21" s="27"/>
       <c r="B21" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
@@ -9296,7 +9287,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
@@ -9316,7 +9307,7 @@
       <c r="A23" s="13"/>
       <c r="B23" s="17"/>
       <c r="C23" s="49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="48"/>
@@ -9346,15 +9337,15 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="10.875" customWidth="1"/>
+    <col min="1" max="256" width="10.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27.95" customHeight="1">
+    <row r="1" spans="1:16" ht="28" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>51</v>
       </c>
@@ -9368,52 +9359,52 @@
         <v>54</v>
       </c>
       <c r="E1" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="G1" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="H1" s="61" t="s">
         <v>152</v>
-      </c>
-      <c r="H1" s="61" t="s">
-        <v>153</v>
       </c>
       <c r="I1" s="61" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="L1" s="52" t="s">
         <v>155</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>156</v>
       </c>
       <c r="M1" s="53"/>
       <c r="N1" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="P1" s="52" t="s">
         <v>158</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="26.25" customHeight="1">
       <c r="A2" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="62" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>123</v>
       </c>
       <c r="C2" s="62" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E2" s="47">
         <v>60</v>
@@ -9428,40 +9419,40 @@
         <v>30</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K2" s="54" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L2" s="54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M2" s="53"/>
       <c r="N2" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O2" s="54" t="s">
+        <v>326</v>
+      </c>
+      <c r="P2" s="55" t="s">
         <v>327</v>
-      </c>
-      <c r="P2" s="55" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
       <c r="A3" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>126</v>
       </c>
       <c r="C3" s="62" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="47">
         <v>60</v>
@@ -9476,40 +9467,40 @@
         <v>30</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J3" s="54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K3" s="54" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L3" s="54" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M3" s="53"/>
       <c r="N3" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O3" s="54" t="s">
+        <v>329</v>
+      </c>
+      <c r="P3" s="55" t="s">
         <v>330</v>
-      </c>
-      <c r="P3" s="55" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>104</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>105</v>
       </c>
       <c r="C4" s="62" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="47">
         <v>40</v>
@@ -9517,29 +9508,47 @@
       <c r="F4" s="47">
         <v>90</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="54"/>
+      <c r="G4" s="47">
+        <v>50</v>
+      </c>
+      <c r="H4" s="47">
+        <v>45</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>336</v>
+      </c>
+      <c r="K4" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="L4" s="54" t="s">
+        <v>332</v>
+      </c>
       <c r="M4" s="53"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="55"/>
+      <c r="N4" s="54" t="s">
+        <v>333</v>
+      </c>
+      <c r="O4" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="P4" s="55" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="A5" s="62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="62" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="47">
         <v>50</v>
@@ -9547,29 +9556,47 @@
       <c r="F5" s="47">
         <v>60</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="54"/>
+      <c r="G5" s="47">
+        <v>29</v>
+      </c>
+      <c r="H5" s="47">
+        <v>20</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>316</v>
+      </c>
+      <c r="K5" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>338</v>
+      </c>
       <c r="M5" s="53"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="55"/>
+      <c r="N5" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="O5" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="P5" s="55" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1">
       <c r="A6" s="62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" s="47">
         <v>50</v>
@@ -9590,16 +9617,16 @@
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E7" s="47">
         <v>50</v>
@@ -9620,10 +9647,10 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>127</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>128</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>38</v>
@@ -9644,23 +9671,23 @@
         <v>20</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J8" s="54" t="s">
+        <v>316</v>
+      </c>
+      <c r="K8" s="56" t="s">
         <v>317</v>
       </c>
-      <c r="K8" s="56" t="s">
-        <v>318</v>
-      </c>
       <c r="L8" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M8" s="53"/>
       <c r="N8" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P8" s="55">
         <v>39</v>
@@ -9668,10 +9695,10 @@
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>129</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>130</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>38</v>
@@ -9692,23 +9719,23 @@
         <v>30</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K9" s="56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M9" s="53"/>
       <c r="N9" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P9" s="55">
         <v>24</v>
@@ -9725,9 +9752,9 @@
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
     </row>
-    <row r="17" spans="3:9" ht="12.95" customHeight="1">
+    <row r="17" spans="3:9" ht="13" customHeight="1">
       <c r="C17" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -9736,7 +9763,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="3:9" ht="12.95" customHeight="1">
+    <row r="18" spans="3:9" ht="13" customHeight="1">
       <c r="C18" s="42"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -9745,12 +9772,12 @@
       <c r="H18" s="19"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="3:9" ht="12.95" customHeight="1">
+    <row r="19" spans="3:9" ht="13" customHeight="1">
       <c r="C19" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>259</v>
+        <v>342</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
@@ -9758,10 +9785,10 @@
       <c r="H19" s="19"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="3:9" ht="12.95" customHeight="1">
+    <row r="20" spans="3:9" ht="13" customHeight="1">
       <c r="C20" s="47"/>
       <c r="D20" s="18" t="s">
-        <v>260</v>
+        <v>343</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
@@ -9769,7 +9796,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="3:9" ht="12.95" customHeight="1">
+    <row r="21" spans="3:9" ht="13" customHeight="1">
       <c r="C21" s="47"/>
       <c r="D21" s="18"/>
       <c r="E21" s="19"/>
@@ -9778,7 +9805,7 @@
       <c r="H21" s="19"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="3:9" ht="12.95" customHeight="1">
+    <row r="22" spans="3:9" ht="13" customHeight="1">
       <c r="C22" s="47"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
@@ -9787,12 +9814,12 @@
       <c r="H22" s="19"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="3:9" ht="12.95" customHeight="1">
+    <row r="23" spans="3:9" ht="13" customHeight="1">
       <c r="C23" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>261</v>
+        <v>344</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -9800,10 +9827,10 @@
       <c r="H23" s="19"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="3:9" ht="12.95" customHeight="1">
+    <row r="24" spans="3:9" ht="13" customHeight="1">
       <c r="C24" s="3"/>
       <c r="D24" s="33" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
@@ -9811,11 +9838,9 @@
       <c r="H24" s="2"/>
       <c r="I24" s="64"/>
     </row>
-    <row r="25" spans="3:9" ht="12.95" customHeight="1">
+    <row r="25" spans="3:9" ht="13" customHeight="1">
       <c r="C25" s="17"/>
-      <c r="D25" s="49" t="s">
-        <v>220</v>
-      </c>
+      <c r="D25" s="49"/>
       <c r="E25" s="13"/>
       <c r="F25" s="48"/>
       <c r="G25" s="48"/>

</xml_diff>

<commit_message>
Added all files and changes - Allan
</commit_message>
<xml_diff>
--- a/Documents/TEAM_AJSV_REPORT.xlsx
+++ b/Documents/TEAM_AJSV_REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -1789,11 +1789,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-49728544"/>
-        <c:axId val="-44364096"/>
+        <c:axId val="-272667104"/>
+        <c:axId val="-272666576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-49728544"/>
+        <c:axId val="-272667104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,14 +1827,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-44364096"/>
+        <c:crossAx val="-272666576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-44364096"/>
+        <c:axId val="-272666576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +1879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-49728544"/>
+        <c:crossAx val="-272667104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -2037,11 +2037,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-49721904"/>
-        <c:axId val="-49718080"/>
+        <c:axId val="-271910352"/>
+        <c:axId val="-271907872"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-49721904"/>
+        <c:axId val="-271910352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2075,14 +2075,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-49718080"/>
+        <c:crossAx val="-271907872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-49718080"/>
+        <c:axId val="-271907872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-49721904"/>
+        <c:crossAx val="-271910352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -4940,7 +4940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5670,7 +5672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="104" workbookViewId="0">
       <selection activeCell="A32" activeCellId="7" sqref="A16 A21 A23 A29 A30 A31 A32 A32"/>
     </sheetView>
   </sheetViews>
@@ -8518,7 +8520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9244,7 +9248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>